<commit_message>
Update spreadsheet of addresses
</commit_message>
<xml_diff>
--- a/Optolink_Logger_v3.xlsx
+++ b/Optolink_Logger_v3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="510" windowWidth="28455" windowHeight="11445"/>
+    <workbookView xWindow="150" yWindow="510" windowWidth="25080" windowHeight="11445"/>
   </bookViews>
   <sheets>
     <sheet name="Datenpunkte" sheetId="1" r:id="rId1"/>
@@ -1314,7 +1314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y135" authorId="1">
+    <comment ref="Y136" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1338,7 +1338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5207" authorId="0">
+    <comment ref="G5208" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1347,42 +1347,6 @@
             <rFont val="Arial"/>
           </rPr>
           <t>Bereich -30 bis 40</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S5207" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Bereich -30 bis 40</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W5207" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Bereich -30 bis 40</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G5208" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Bereich 0.2 bis 3.5</t>
         </r>
       </text>
     </comment>
@@ -1394,11 +1358,47 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Bereich 0.2 bis 3.5</t>
+          <t>Bereich -30 bis 40</t>
         </r>
       </text>
     </comment>
     <comment ref="W5208" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Bereich -30 bis 40</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5209" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Bereich 0.2 bis 3.5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S5209" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Bereich 0.2 bis 3.5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W5209" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1415,7 +1415,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="459">
   <si>
     <t>V333MW1</t>
   </si>
@@ -2347,15 +2347,6 @@
     <t>Return / flow temperature (17B) low-pass</t>
   </si>
   <si>
-    <t>Room temperature A1M1 low-pass</t>
-  </si>
-  <si>
-    <t>Room temperature M2 lowpass</t>
-  </si>
-  <si>
-    <t>Room temperature M3 low-pass</t>
-  </si>
-  <si>
     <t>Maximum exhaust temperature reached</t>
   </si>
   <si>
@@ -2396,9 +2387,6 @@
   </si>
   <si>
     <t>States of pumps, mixers, etc.</t>
-  </si>
-  <si>
-    <t>circulation pump</t>
   </si>
   <si>
     <t>Mixer M1 position (0 to 100%)</t>
@@ -2492,12 +2480,6 @@
     <t>Hot water temperature (sensor 5)</t>
   </si>
   <si>
-    <t>Hot Water temperature low-pass</t>
-  </si>
-  <si>
-    <t>Hot Water temperature for 2 low-pass</t>
-  </si>
-  <si>
     <t>Hot water tank charging pump</t>
   </si>
   <si>
@@ -2541,9 +2523,6 @@
   </si>
   <si>
     <t>getBoilerTempLP</t>
-  </si>
-  <si>
-    <t>getRoomTempLP</t>
   </si>
   <si>
     <t>getFlowTemp</t>
@@ -2688,9 +2667,6 @@
     <t>SetReducedTempSP</t>
   </si>
   <si>
-    <t>Set hot Water temperature setpoint</t>
-  </si>
-  <si>
     <t>0x6300</t>
   </si>
   <si>
@@ -2728,6 +2704,105 @@
   </si>
   <si>
     <t>bit</t>
+  </si>
+  <si>
+    <t>0..64</t>
+  </si>
+  <si>
+    <t>getCurrentOpMode1</t>
+  </si>
+  <si>
+    <t>getFlowTemp1</t>
+  </si>
+  <si>
+    <t>getCircPumpStatus1</t>
+  </si>
+  <si>
+    <t>getRoomTemp1</t>
+  </si>
+  <si>
+    <t>getCurrentOpMode2</t>
+  </si>
+  <si>
+    <t>getFlowTemp2</t>
+  </si>
+  <si>
+    <t>getCircPumpStatus2</t>
+  </si>
+  <si>
+    <t>getRoomTemp2</t>
+  </si>
+  <si>
+    <t>getCurrentOpMode3</t>
+  </si>
+  <si>
+    <t>getFlowTemp3</t>
+  </si>
+  <si>
+    <t>getCircPumpStatus3</t>
+  </si>
+  <si>
+    <t>getRoomTemp3</t>
+  </si>
+  <si>
+    <t>Hot Water temperature (CTS1)</t>
+  </si>
+  <si>
+    <t>Hot Water temperature (CTS2)</t>
+  </si>
+  <si>
+    <t>getHotWaterTemp1</t>
+  </si>
+  <si>
+    <t>getHotWaterTemp2</t>
+  </si>
+  <si>
+    <t>DHW circulation pump</t>
+  </si>
+  <si>
+    <t>0..127</t>
+  </si>
+  <si>
+    <t>Flow temperature M1 setpoint (read)</t>
+  </si>
+  <si>
+    <t>Flow temperature M2 setpoint (read)</t>
+  </si>
+  <si>
+    <t>Flow temperature M3 setpoint (read)</t>
+  </si>
+  <si>
+    <t>getFlowTempSP1</t>
+  </si>
+  <si>
+    <t>getFlowTempSP2</t>
+  </si>
+  <si>
+    <t>getFlowTempSP3</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Set Hot Water temperature setpoint</t>
+  </si>
+  <si>
+    <t>getBurnerStage1</t>
+  </si>
+  <si>
+    <t>getBurnerStage2</t>
+  </si>
+  <si>
+    <t>0..500</t>
   </si>
 </sst>
 </file>
@@ -2737,7 +2812,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2876,6 +2951,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -2963,7 +3052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3001,13 +3090,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3038,8 +3125,8 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3053,6 +3140,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3347,13 +3439,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AQ5208"/>
+  <dimension ref="B1:AR5209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V122" sqref="V122"/>
+      <selection pane="bottomRight" activeCell="AS91" sqref="AS91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -3402,7 +3494,7 @@
     <col min="42" max="42" width="1.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" ht="18" customHeight="1">
+    <row r="1" spans="2:44" ht="18" customHeight="1">
       <c r="B1" s="10" t="s">
         <v>281</v>
       </c>
@@ -3446,54 +3538,54 @@
       <c r="AO1" s="15"/>
       <c r="AP1" s="15"/>
     </row>
-    <row r="2" spans="2:42">
-      <c r="E2" s="25" t="s">
+    <row r="2" spans="2:44" ht="21.75" customHeight="1">
+      <c r="E2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="I2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="M2" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="Q2" s="25" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="I2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="M2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="Q2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="U2" s="25" t="s">
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="U2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="AA2" s="25" t="s">
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="AA2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AE2" s="27" t="s">
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AE2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="27"/>
-      <c r="AI2" s="27" t="s">
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AI2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AM2" s="27" t="s">
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AM2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-    </row>
-    <row r="3" spans="2:42" ht="1.5" customHeight="1">
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="26"/>
+    </row>
+    <row r="3" spans="2:44" ht="21.75" customHeight="1">
       <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3579,8 +3671,14 @@
       <c r="AO3" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:42" ht="25.5">
+      <c r="AQ3" s="22" t="s">
+        <v>453</v>
+      </c>
+      <c r="AR3" s="22" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="4" spans="2:44" ht="21.75" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>282</v>
       </c>
@@ -3629,11 +3727,11 @@
       <c r="W4" s="1">
         <v>2</v>
       </c>
-      <c r="X4" s="20" t="s">
-        <v>359</v>
+      <c r="X4" s="19" t="s">
+        <v>353</v>
       </c>
       <c r="Y4" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA4" s="7" t="s">
         <v>12</v>
@@ -3666,16 +3764,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:42" ht="12.75" customHeight="1">
-      <c r="X5" s="20"/>
-    </row>
-    <row r="6" spans="2:42" ht="12.75" customHeight="1">
+    <row r="5" spans="2:44" ht="12.75" customHeight="1">
+      <c r="X5" s="19"/>
+    </row>
+    <row r="6" spans="2:44" ht="12.75" customHeight="1">
       <c r="B6" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="X6" s="20"/>
-    </row>
-    <row r="7" spans="2:42" ht="12.75" customHeight="1">
+      <c r="X6" s="19"/>
+    </row>
+    <row r="7" spans="2:44" ht="12.75" customHeight="1">
       <c r="B7" s="7" t="s">
         <v>284</v>
       </c>
@@ -3709,11 +3807,11 @@
       <c r="W7" s="7">
         <v>2</v>
       </c>
-      <c r="X7" s="21" t="s">
-        <v>361</v>
+      <c r="X7" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="Y7" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AI7" t="s">
         <v>24</v>
@@ -3734,7 +3832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:42" ht="12.75" customHeight="1">
+    <row r="8" spans="2:44" ht="12.75" customHeight="1">
       <c r="B8" s="7" t="s">
         <v>285</v>
       </c>
@@ -3777,16 +3875,16 @@
       <c r="W8" s="7">
         <v>2</v>
       </c>
-      <c r="X8" s="21" t="s">
-        <v>362</v>
+      <c r="X8" s="20" t="s">
+        <v>356</v>
       </c>
       <c r="Y8" s="8" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="9" spans="2:42" ht="12.75" customHeight="1">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="9" spans="2:44" ht="12.75" customHeight="1">
       <c r="B9" s="8" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>27</v>
@@ -3827,11 +3925,11 @@
       <c r="W9" s="7">
         <v>2</v>
       </c>
-      <c r="X9" s="21" t="s">
-        <v>363</v>
+      <c r="X9" s="20" t="s">
+        <v>357</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AI9" t="s">
         <v>29</v>
@@ -3852,7 +3950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:42" ht="12.75" customHeight="1">
+    <row r="10" spans="2:44" ht="12.75" customHeight="1">
       <c r="B10" s="7" t="s">
         <v>286</v>
       </c>
@@ -3886,7 +3984,7 @@
       <c r="S10" s="7">
         <v>2</v>
       </c>
-      <c r="X10" s="20"/>
+      <c r="X10" s="19"/>
       <c r="AA10" s="4" t="s">
         <v>31</v>
       </c>
@@ -3906,7 +4004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:42" ht="12.75" customHeight="1">
+    <row r="11" spans="2:44" ht="12.75" customHeight="1">
       <c r="B11" s="7" t="s">
         <v>287</v>
       </c>
@@ -3917,7 +4015,7 @@
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
-      <c r="X11" s="20"/>
+      <c r="X11" s="19"/>
       <c r="AA11" s="8"/>
       <c r="AB11" s="8"/>
       <c r="AC11" s="8"/>
@@ -3931,7 +4029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:42" ht="12.75" customHeight="1">
+    <row r="12" spans="2:44" ht="12.75" customHeight="1">
       <c r="B12" s="7" t="s">
         <v>288</v>
       </c>
@@ -3942,7 +4040,7 @@
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
-      <c r="X12" s="20"/>
+      <c r="X12" s="19"/>
       <c r="AA12" s="8"/>
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
@@ -3956,7 +4054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:42" ht="12.75" customHeight="1">
+    <row r="13" spans="2:44" ht="12.75" customHeight="1">
       <c r="B13" s="7" t="s">
         <v>289</v>
       </c>
@@ -3981,20 +4079,20 @@
       <c r="S13" s="7">
         <v>2</v>
       </c>
-      <c r="U13" s="17" t="s">
-        <v>406</v>
-      </c>
-      <c r="V13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W13" s="7">
-        <v>2</v>
-      </c>
-      <c r="X13" s="21" t="s">
-        <v>364</v>
+      <c r="U13" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="V13" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="W13" s="33">
+        <v>2</v>
+      </c>
+      <c r="X13" s="34" t="s">
+        <v>358</v>
       </c>
       <c r="Y13" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA13" s="7" t="s">
         <v>35</v>
@@ -4014,8 +4112,11 @@
       <c r="AO13" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="2:42" ht="12.75" customHeight="1">
+      <c r="AQ13" s="22" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="14" spans="2:44" ht="12.75" customHeight="1">
       <c r="B14" s="7" t="s">
         <v>290</v>
       </c>
@@ -4067,14 +4168,14 @@
       <c r="W14" s="7">
         <v>2</v>
       </c>
-      <c r="X14" s="21" t="s">
-        <v>365</v>
+      <c r="X14" s="45" t="s">
+        <v>359</v>
       </c>
       <c r="Y14" s="8" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="15" spans="2:42" ht="12.75" customHeight="1">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="15" spans="2:44" ht="12.75" customHeight="1">
       <c r="B15" s="7" t="s">
         <v>291</v>
       </c>
@@ -4117,14 +4218,14 @@
       <c r="W15" s="7">
         <v>2</v>
       </c>
-      <c r="X15" s="21" t="s">
-        <v>366</v>
+      <c r="X15" s="45" t="s">
+        <v>360</v>
       </c>
       <c r="Y15" s="8" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="16" spans="2:42" ht="12.75" customHeight="1">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="16" spans="2:44" ht="12.75" customHeight="1">
       <c r="B16" s="7" t="s">
         <v>292</v>
       </c>
@@ -4137,7 +4238,7 @@
       <c r="G16" s="7">
         <v>2</v>
       </c>
-      <c r="X16" s="20"/>
+      <c r="X16" s="19"/>
       <c r="AI16" t="s">
         <v>41</v>
       </c>
@@ -4188,11 +4289,11 @@
       <c r="W17" s="7">
         <v>2</v>
       </c>
-      <c r="X17" s="36" t="s">
-        <v>367</v>
+      <c r="X17" s="34" t="s">
+        <v>361</v>
       </c>
       <c r="Y17" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA17" s="7" t="s">
         <v>42</v>
@@ -4262,11 +4363,11 @@
       <c r="W18" s="7">
         <v>2</v>
       </c>
-      <c r="X18" s="21" t="s">
-        <v>368</v>
+      <c r="X18" s="20" t="s">
+        <v>362</v>
       </c>
       <c r="Y18" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA18" s="7" t="s">
         <v>44</v>
@@ -4300,7 +4401,7 @@
       <c r="G19" s="7">
         <v>2</v>
       </c>
-      <c r="X19" s="20"/>
+      <c r="X19" s="19"/>
     </row>
     <row r="20" spans="2:41" ht="12.75" customHeight="1">
       <c r="B20" s="7" t="s">
@@ -4315,7 +4416,7 @@
       <c r="G20" s="7">
         <v>2</v>
       </c>
-      <c r="X20" s="20"/>
+      <c r="X20" s="19"/>
     </row>
     <row r="21" spans="2:41" ht="12.75" customHeight="1">
       <c r="B21" s="7" t="s">
@@ -4330,7 +4431,7 @@
       <c r="G21" s="7">
         <v>2</v>
       </c>
-      <c r="X21" s="20"/>
+      <c r="X21" s="19"/>
     </row>
     <row r="22" spans="2:41" ht="12.75" customHeight="1">
       <c r="B22" s="7" t="s">
@@ -4345,7 +4446,7 @@
       <c r="G22" s="7">
         <v>2</v>
       </c>
-      <c r="X22" s="20"/>
+      <c r="X22" s="19"/>
     </row>
     <row r="23" spans="2:41" ht="12.75" customHeight="1">
       <c r="B23" s="7" t="s">
@@ -4360,7 +4461,7 @@
       <c r="G23" s="7">
         <v>2</v>
       </c>
-      <c r="X23" s="20"/>
+      <c r="X23" s="19"/>
       <c r="AM23" t="s">
         <v>50</v>
       </c>
@@ -4402,7 +4503,7 @@
       <c r="W24" s="7">
         <v>2</v>
       </c>
-      <c r="X24" s="21"/>
+      <c r="X24" s="20"/>
       <c r="Y24" s="7"/>
       <c r="AA24" s="7" t="s">
         <v>51</v>
@@ -4445,7 +4546,7 @@
       <c r="G25" s="7">
         <v>2</v>
       </c>
-      <c r="X25" s="20"/>
+      <c r="X25" s="19"/>
       <c r="AI25" t="s">
         <v>54</v>
       </c>
@@ -4469,7 +4570,7 @@
       <c r="W26" s="7">
         <v>2</v>
       </c>
-      <c r="X26" s="21"/>
+      <c r="X26" s="20"/>
       <c r="Y26" s="7"/>
     </row>
     <row r="27" spans="2:41" ht="12.75" customHeight="1">
@@ -4512,15 +4613,15 @@
       <c r="W27" s="7">
         <v>2</v>
       </c>
-      <c r="X27" s="21" t="s">
-        <v>370</v>
+      <c r="X27" s="20" t="s">
+        <v>364</v>
       </c>
       <c r="Y27" s="8" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="2:41" ht="12.75" customHeight="1">
-      <c r="X28" s="20"/>
+      <c r="X28" s="19"/>
     </row>
     <row r="29" spans="2:41" ht="12.75" customHeight="1">
       <c r="B29" s="7" t="s">
@@ -4562,20 +4663,18 @@
       <c r="S29" s="7">
         <v>2</v>
       </c>
-      <c r="U29" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="U29" s="16"/>
       <c r="V29" s="7" t="s">
         <v>23</v>
       </c>
       <c r="W29" s="7">
         <v>2</v>
       </c>
-      <c r="X29" s="36" t="s">
-        <v>372</v>
+      <c r="X29" s="43" t="s">
+        <v>366</v>
       </c>
       <c r="Y29" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA29" s="7" t="s">
         <v>58</v>
@@ -4597,8 +4696,8 @@
       </c>
     </row>
     <row r="30" spans="2:41" ht="12.75" customHeight="1">
-      <c r="B30" s="8" t="s">
-        <v>356</v>
+      <c r="B30" s="21" t="s">
+        <v>439</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>27</v>
@@ -4639,16 +4738,18 @@
       <c r="S30" s="7">
         <v>2</v>
       </c>
-      <c r="U30" s="7" t="s">
+      <c r="U30" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="V30" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W30" s="7">
-        <v>2</v>
-      </c>
-      <c r="X30" s="21"/>
+      <c r="V30" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="W30" s="17">
+        <v>2</v>
+      </c>
+      <c r="X30" s="34" t="s">
+        <v>441</v>
+      </c>
       <c r="Y30" s="7"/>
       <c r="AA30" s="7" t="s">
         <v>59</v>
@@ -4679,8 +4780,8 @@
       </c>
     </row>
     <row r="31" spans="2:41" ht="12.75" customHeight="1">
-      <c r="B31" s="8" t="s">
-        <v>357</v>
+      <c r="B31" s="21" t="s">
+        <v>440</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>30</v>
@@ -4721,16 +4822,18 @@
       <c r="S31" s="7">
         <v>2</v>
       </c>
-      <c r="U31" s="7" t="s">
+      <c r="U31" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="V31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W31" s="7">
-        <v>2</v>
-      </c>
-      <c r="X31" s="21"/>
+      <c r="V31" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="W31" s="17">
+        <v>2</v>
+      </c>
+      <c r="X31" s="34" t="s">
+        <v>442</v>
+      </c>
       <c r="Y31" s="7"/>
       <c r="AA31" s="7" t="s">
         <v>60</v>
@@ -4788,7 +4891,7 @@
       <c r="W32" s="7">
         <v>2</v>
       </c>
-      <c r="X32" s="21"/>
+      <c r="X32" s="20"/>
       <c r="Y32" s="7"/>
       <c r="AE32" s="7" t="s">
         <v>61</v>
@@ -4800,7 +4903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:37" ht="12.75" customHeight="1">
+    <row r="33" spans="2:43" ht="12.75" customHeight="1">
       <c r="B33" s="7" t="s">
         <v>306</v>
       </c>
@@ -4831,16 +4934,18 @@
       <c r="S33" s="7">
         <v>2</v>
       </c>
-      <c r="U33" s="7" t="s">
+      <c r="U33" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="V33" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W33" s="7">
-        <v>2</v>
-      </c>
-      <c r="X33" s="21"/>
+      <c r="V33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="W33" s="17">
+        <v>2</v>
+      </c>
+      <c r="X33" s="34" t="s">
+        <v>359</v>
+      </c>
       <c r="Y33" s="7"/>
       <c r="AE33" s="7" t="s">
         <v>62</v>
@@ -4851,8 +4956,11 @@
       <c r="AG33" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="2:37" ht="12.75" customHeight="1">
+      <c r="AQ33" s="22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="34" spans="2:43" ht="12.75" customHeight="1">
       <c r="B34" s="7" t="s">
         <v>307</v>
       </c>
@@ -4883,21 +4991,26 @@
       <c r="S34" s="7">
         <v>2</v>
       </c>
-      <c r="U34" s="7" t="s">
+      <c r="U34" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="V34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W34" s="7">
-        <v>2</v>
-      </c>
-      <c r="X34" s="21"/>
+      <c r="V34" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="W34" s="17">
+        <v>2</v>
+      </c>
+      <c r="X34" s="34" t="s">
+        <v>360</v>
+      </c>
       <c r="Y34" s="7"/>
-    </row>
-    <row r="35" spans="2:37" ht="12.75" customHeight="1">
-      <c r="B35" s="7" t="s">
-        <v>308</v>
+      <c r="AQ34" s="22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="35" spans="2:43" ht="12.75" customHeight="1">
+      <c r="B35" s="21" t="s">
+        <v>445</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>64</v>
@@ -4920,8 +5033,8 @@
       <c r="S35" s="7">
         <v>2</v>
       </c>
-      <c r="U35" s="17" t="s">
-        <v>65</v>
+      <c r="U35" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>23</v>
@@ -4929,11 +5042,11 @@
       <c r="W35" s="7">
         <v>2</v>
       </c>
-      <c r="X35" s="21" t="s">
-        <v>373</v>
+      <c r="X35" s="34" t="s">
+        <v>448</v>
       </c>
       <c r="Y35" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA35" s="7" t="s">
         <v>65</v>
@@ -4944,10 +5057,13 @@
       <c r="AC35" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:37" ht="12.75" customHeight="1">
-      <c r="B36" s="7" t="s">
-        <v>309</v>
+      <c r="AQ35" s="22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="36" spans="2:43" ht="12.75" customHeight="1">
+      <c r="B36" s="21" t="s">
+        <v>446</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>66</v>
@@ -4961,7 +5077,18 @@
       <c r="G36" s="7">
         <v>2</v>
       </c>
-      <c r="X36" s="20"/>
+      <c r="U36" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="V36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="W36" s="7">
+        <v>2</v>
+      </c>
+      <c r="X36" s="44" t="s">
+        <v>449</v>
+      </c>
       <c r="AA36" s="7" t="s">
         <v>67</v>
       </c>
@@ -4971,10 +5098,13 @@
       <c r="AC36" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="2:37" ht="12.75" customHeight="1">
-      <c r="B37" s="7" t="s">
-        <v>310</v>
+      <c r="AQ36" s="22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="37" spans="2:43" ht="12.75" customHeight="1">
+      <c r="B37" s="21" t="s">
+        <v>447</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>68</v>
@@ -4985,11 +5115,25 @@
       <c r="G37" s="7">
         <v>2</v>
       </c>
-      <c r="X37" s="20"/>
-    </row>
-    <row r="38" spans="2:37" ht="12.75" customHeight="1">
+      <c r="U37" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="V37" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="W37" s="21">
+        <v>2</v>
+      </c>
+      <c r="X37" s="44" t="s">
+        <v>450</v>
+      </c>
+      <c r="AQ37" s="22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="38" spans="2:43" ht="12.75" customHeight="1">
       <c r="B38" s="7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>69</v>
@@ -5018,19 +5162,19 @@
       <c r="W38" s="7">
         <v>2</v>
       </c>
-      <c r="X38" s="21"/>
+      <c r="X38" s="20"/>
       <c r="Y38" s="7"/>
     </row>
-    <row r="39" spans="2:37" ht="12.75" customHeight="1">
-      <c r="X39" s="20"/>
-    </row>
-    <row r="40" spans="2:37" ht="12.75" customHeight="1">
+    <row r="39" spans="2:43" ht="12.75" customHeight="1">
+      <c r="X39" s="19"/>
+    </row>
+    <row r="40" spans="2:43" ht="12.75" customHeight="1">
       <c r="B40" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="X40" s="20"/>
-    </row>
-    <row r="41" spans="2:37" ht="12.75" customHeight="1">
+        <v>309</v>
+      </c>
+      <c r="X40" s="19"/>
+    </row>
+    <row r="41" spans="2:43" ht="12.75" customHeight="1">
       <c r="B41" s="7" t="s">
         <v>292</v>
       </c>
@@ -5043,9 +5187,9 @@
       <c r="G41" s="7">
         <v>2</v>
       </c>
-      <c r="X41" s="20"/>
-    </row>
-    <row r="42" spans="2:37" ht="12.75" customHeight="1">
+      <c r="X41" s="19"/>
+    </row>
+    <row r="42" spans="2:43" ht="12.75" customHeight="1">
       <c r="B42" s="7" t="s">
         <v>299</v>
       </c>
@@ -5085,8 +5229,8 @@
       <c r="S42" s="7">
         <v>2</v>
       </c>
-      <c r="U42" s="17" t="s">
-        <v>71</v>
+      <c r="U42" s="33" t="s">
+        <v>58</v>
       </c>
       <c r="V42" s="7" t="s">
         <v>23</v>
@@ -5094,11 +5238,11 @@
       <c r="W42" s="7">
         <v>2</v>
       </c>
-      <c r="X42" s="21" t="s">
-        <v>374</v>
+      <c r="X42" s="34" t="s">
+        <v>367</v>
       </c>
       <c r="Y42" s="8" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="AA42" s="7" t="s">
         <v>71</v>
@@ -5110,11 +5254,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:37" ht="12.75" customHeight="1">
+    <row r="43" spans="2:43" ht="12.75" customHeight="1">
       <c r="B43" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="X43" s="20"/>
+        <v>310</v>
+      </c>
+      <c r="X43" s="19"/>
       <c r="AA43" s="7" t="s">
         <v>72</v>
       </c>
@@ -5125,7 +5269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:37" ht="12.75" customHeight="1">
+    <row r="44" spans="2:43" ht="12.75" customHeight="1">
       <c r="B44" s="7" t="s">
         <v>300</v>
       </c>
@@ -5147,7 +5291,7 @@
       <c r="O44" s="7">
         <v>2</v>
       </c>
-      <c r="X44" s="20"/>
+      <c r="X44" s="19"/>
       <c r="AA44" s="7" t="s">
         <v>73</v>
       </c>
@@ -5158,7 +5302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:37" ht="12.75" customHeight="1">
+    <row r="45" spans="2:43" ht="12.75" customHeight="1">
       <c r="B45" s="7" t="s">
         <v>301</v>
       </c>
@@ -5171,7 +5315,7 @@
       <c r="G45" s="7">
         <v>2</v>
       </c>
-      <c r="X45" s="20"/>
+      <c r="X45" s="19"/>
       <c r="AI45" t="s">
         <v>75</v>
       </c>
@@ -5182,9 +5326,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:37" ht="12.75" customHeight="1">
+    <row r="46" spans="2:43" ht="12.75" customHeight="1">
       <c r="B46" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>76</v>
@@ -5195,11 +5339,11 @@
       <c r="G46" s="7">
         <v>2</v>
       </c>
-      <c r="X46" s="20"/>
-    </row>
-    <row r="47" spans="2:37" ht="12.75" customHeight="1">
+      <c r="X46" s="19"/>
+    </row>
+    <row r="47" spans="2:43" ht="12.75" customHeight="1">
       <c r="B47" s="7" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>77</v>
@@ -5228,20 +5372,20 @@
       <c r="S47" s="7">
         <v>2</v>
       </c>
-      <c r="U47" s="17" t="s">
+      <c r="U47" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="V47" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W47" s="7">
-        <v>2</v>
-      </c>
-      <c r="X47" s="21" t="s">
-        <v>369</v>
+      <c r="V47" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="W47" s="33">
+        <v>2</v>
+      </c>
+      <c r="X47" s="34" t="s">
+        <v>363</v>
       </c>
       <c r="Y47" s="8" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="AA47" s="7" t="s">
         <v>77</v>
@@ -5261,8 +5405,11 @@
       <c r="AG47" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="2:37" ht="12.75" customHeight="1">
+      <c r="AQ47" s="22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="48" spans="2:43" ht="12.75" customHeight="1">
       <c r="B48" s="7" t="s">
         <v>295</v>
       </c>
@@ -5275,9 +5422,9 @@
       <c r="G48" s="7">
         <v>2</v>
       </c>
-      <c r="X48" s="20"/>
-    </row>
-    <row r="49" spans="2:41" ht="12.75" customHeight="1">
+      <c r="X48" s="19"/>
+    </row>
+    <row r="49" spans="2:43" ht="12.75" customHeight="1">
       <c r="B49" s="7" t="s">
         <v>296</v>
       </c>
@@ -5290,9 +5437,9 @@
       <c r="G49" s="7">
         <v>2</v>
       </c>
-      <c r="X49" s="20"/>
-    </row>
-    <row r="50" spans="2:41" ht="12.75" customHeight="1">
+      <c r="X49" s="19"/>
+    </row>
+    <row r="50" spans="2:43" ht="12.75" customHeight="1">
       <c r="B50" s="7" t="s">
         <v>297</v>
       </c>
@@ -5305,9 +5452,9 @@
       <c r="G50" s="7">
         <v>2</v>
       </c>
-      <c r="X50" s="20"/>
-    </row>
-    <row r="51" spans="2:41" ht="12.75" customHeight="1">
+      <c r="X50" s="19"/>
+    </row>
+    <row r="51" spans="2:43" ht="12.75" customHeight="1">
       <c r="B51" s="7" t="s">
         <v>298</v>
       </c>
@@ -5320,20 +5467,20 @@
       <c r="G51" s="7">
         <v>2</v>
       </c>
-      <c r="X51" s="20"/>
-    </row>
-    <row r="52" spans="2:41" ht="12.75" customHeight="1">
-      <c r="X52" s="20"/>
-    </row>
-    <row r="53" spans="2:41" ht="12.75" customHeight="1">
+      <c r="X51" s="19"/>
+    </row>
+    <row r="52" spans="2:43" ht="12.75" customHeight="1">
+      <c r="X52" s="19"/>
+    </row>
+    <row r="53" spans="2:43" ht="12.75" customHeight="1">
       <c r="B53" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="X53" s="20"/>
-    </row>
-    <row r="54" spans="2:41" ht="12.75" customHeight="1">
+        <v>313</v>
+      </c>
+      <c r="X53" s="19"/>
+    </row>
+    <row r="54" spans="2:43" ht="12.75" customHeight="1">
       <c r="B54" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="I54" s="7" t="s">
         <v>82</v>
@@ -5362,12 +5509,12 @@
       <c r="W54" s="7">
         <v>1</v>
       </c>
-      <c r="X54" s="21"/>
+      <c r="X54" s="20"/>
       <c r="Y54" s="7"/>
     </row>
-    <row r="55" spans="2:41" ht="12.75" customHeight="1">
+    <row r="55" spans="2:43" ht="12.75" customHeight="1">
       <c r="B55" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I55" s="7" t="s">
         <v>84</v>
@@ -5396,11 +5543,11 @@
       <c r="W55" s="7">
         <v>1</v>
       </c>
-      <c r="X55" s="21" t="s">
-        <v>375</v>
+      <c r="X55" s="20" t="s">
+        <v>368</v>
       </c>
       <c r="Y55" s="8" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="AA55" s="7" t="s">
         <v>86</v>
@@ -5412,9 +5559,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:41" ht="12.75" customHeight="1">
+    <row r="56" spans="2:43" ht="12.75" customHeight="1">
       <c r="B56" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I56" s="7" t="s">
         <v>87</v>
@@ -5443,12 +5590,12 @@
       <c r="W56" s="7">
         <v>1</v>
       </c>
-      <c r="X56" s="21"/>
+      <c r="X56" s="20"/>
       <c r="Y56" s="7"/>
     </row>
-    <row r="57" spans="2:41" ht="12.75" customHeight="1">
-      <c r="B57" s="22" t="s">
-        <v>403</v>
+    <row r="57" spans="2:43" ht="12.75" customHeight="1">
+      <c r="B57" s="21" t="s">
+        <v>396</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>89</v>
@@ -5468,21 +5615,26 @@
       <c r="S57" s="7">
         <v>1</v>
       </c>
-      <c r="U57" s="37" t="s">
-        <v>402</v>
-      </c>
-      <c r="V57" s="17" t="s">
+      <c r="U57" s="35" t="s">
+        <v>395</v>
+      </c>
+      <c r="V57" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="W57" s="33">
+        <v>1</v>
+      </c>
+      <c r="X57" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="Y57" s="7"/>
+      <c r="AQ57" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="W57" s="17">
-        <v>1</v>
-      </c>
-      <c r="X57" s="21"/>
-      <c r="Y57" s="7"/>
-    </row>
-    <row r="58" spans="2:41" ht="12.75" customHeight="1">
-      <c r="B58" s="22" t="s">
-        <v>404</v>
+    </row>
+    <row r="58" spans="2:43" ht="12.75" customHeight="1">
+      <c r="B58" s="21" t="s">
+        <v>397</v>
       </c>
       <c r="I58" s="7" t="s">
         <v>90</v>
@@ -5502,21 +5654,26 @@
       <c r="S58" s="7">
         <v>1</v>
       </c>
-      <c r="U58" s="37" t="s">
-        <v>405</v>
-      </c>
-      <c r="V58" s="17" t="s">
+      <c r="U58" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="V58" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="W58" s="33">
+        <v>1</v>
+      </c>
+      <c r="X58" s="34" t="s">
+        <v>457</v>
+      </c>
+      <c r="Y58" s="7"/>
+      <c r="AQ58" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="W58" s="17">
-        <v>1</v>
-      </c>
-      <c r="X58" s="21"/>
-      <c r="Y58" s="7"/>
-    </row>
-    <row r="59" spans="2:41" ht="12.75" customHeight="1">
+    </row>
+    <row r="59" spans="2:43" ht="12.75" customHeight="1">
       <c r="B59" s="7" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>91</v>
@@ -5545,16 +5702,16 @@
       <c r="W59" s="7">
         <v>4</v>
       </c>
-      <c r="X59" s="21" t="s">
-        <v>376</v>
+      <c r="X59" s="20" t="s">
+        <v>369</v>
       </c>
       <c r="Y59" s="8" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="60" spans="2:41" ht="12.75" customHeight="1">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="60" spans="2:43" ht="12.75" customHeight="1">
       <c r="B60" s="6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>93</v>
@@ -5580,11 +5737,11 @@
       <c r="W60" s="7">
         <v>4</v>
       </c>
-      <c r="X60" s="36" t="s">
-        <v>377</v>
+      <c r="X60" s="34" t="s">
+        <v>370</v>
       </c>
       <c r="Y60" s="8" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="AA60" s="7" t="s">
         <v>93</v>
@@ -5605,9 +5762,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="2:41" ht="12.75" customHeight="1">
+    <row r="61" spans="2:43" ht="12.75" customHeight="1">
       <c r="B61" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>94</v>
@@ -5645,11 +5802,11 @@
       <c r="W61" s="17">
         <v>4</v>
       </c>
-      <c r="X61" s="36" t="s">
-        <v>378</v>
+      <c r="X61" s="34" t="s">
+        <v>371</v>
       </c>
       <c r="Y61" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA61" s="7" t="s">
         <v>96</v>
@@ -5679,9 +5836,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="2:41" ht="12.75" customHeight="1">
+    <row r="62" spans="2:43" ht="12.75" customHeight="1">
       <c r="B62" s="6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="I62" s="7" t="s">
         <v>97</v>
@@ -5710,28 +5867,28 @@
       <c r="W62" s="17">
         <v>4</v>
       </c>
-      <c r="X62" s="36" t="s">
+      <c r="X62" s="34" t="s">
+        <v>372</v>
+      </c>
+      <c r="Y62" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="63" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+      <c r="X63" s="19"/>
+    </row>
+    <row r="64" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+      <c r="B64" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="28"/>
+      <c r="X64" s="19"/>
+    </row>
+    <row r="65" spans="2:41" ht="12.75" hidden="1" customHeight="1">
+      <c r="B65" s="29" t="s">
         <v>379</v>
       </c>
-      <c r="Y62" s="8" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="63" spans="2:41" ht="12.75" hidden="1" customHeight="1">
-      <c r="X63" s="20"/>
-    </row>
-    <row r="64" spans="2:41" ht="12.75" hidden="1" customHeight="1">
-      <c r="B64" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="C64" s="30"/>
-      <c r="X64" s="20"/>
-    </row>
-    <row r="65" spans="2:41" ht="12.75" hidden="1" customHeight="1">
-      <c r="B65" s="31" t="s">
-        <v>386</v>
-      </c>
-      <c r="C65" s="32"/>
+      <c r="C65" s="30"/>
       <c r="M65" s="7" t="s">
         <v>100</v>
       </c>
@@ -5741,7 +5898,7 @@
       <c r="O65" s="7">
         <v>2</v>
       </c>
-      <c r="X65" s="20"/>
+      <c r="X65" s="19"/>
       <c r="AA65" s="7" t="s">
         <v>100</v>
       </c>
@@ -5771,17 +5928,17 @@
       </c>
     </row>
     <row r="66" spans="2:41" ht="12.75" hidden="1" customHeight="1">
-      <c r="B66" s="33" t="s">
-        <v>389</v>
-      </c>
-      <c r="C66" s="30"/>
+      <c r="B66" s="31" t="s">
+        <v>382</v>
+      </c>
+      <c r="C66" s="28"/>
       <c r="M66" s="7" t="s">
         <v>102</v>
       </c>
       <c r="O66" s="7">
         <v>2</v>
       </c>
-      <c r="X66" s="20"/>
+      <c r="X66" s="19"/>
       <c r="AA66" s="7" t="s">
         <v>102</v>
       </c>
@@ -5808,7 +5965,7 @@
       <c r="O67" s="7">
         <v>1</v>
       </c>
-      <c r="X67" s="20"/>
+      <c r="X67" s="19"/>
       <c r="AA67" s="7" t="s">
         <v>104</v>
       </c>
@@ -5821,7 +5978,7 @@
     </row>
     <row r="68" spans="2:41" ht="12.75" hidden="1" customHeight="1">
       <c r="B68" s="7" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="M68" s="7" t="s">
         <v>105</v>
@@ -5832,7 +5989,7 @@
       <c r="O68" s="7">
         <v>1</v>
       </c>
-      <c r="X68" s="20"/>
+      <c r="X68" s="19"/>
       <c r="AA68" s="7" t="s">
         <v>105</v>
       </c>
@@ -5845,7 +6002,7 @@
     </row>
     <row r="69" spans="2:41" ht="12.75" hidden="1" customHeight="1">
       <c r="B69" s="7" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="M69" s="7" t="s">
         <v>106</v>
@@ -5856,7 +6013,7 @@
       <c r="O69" s="7">
         <v>2</v>
       </c>
-      <c r="X69" s="20"/>
+      <c r="X69" s="19"/>
       <c r="AA69" s="7" t="s">
         <v>106</v>
       </c>
@@ -5883,7 +6040,7 @@
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
       <c r="O70" s="7"/>
-      <c r="X70" s="20"/>
+      <c r="X70" s="19"/>
       <c r="AA70" s="7"/>
       <c r="AB70" s="7"/>
       <c r="AC70" s="7"/>
@@ -5899,7 +6056,7 @@
     </row>
     <row r="71" spans="2:41" ht="12.75" hidden="1" customHeight="1">
       <c r="B71" s="6" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="M71" s="7" t="s">
         <v>109</v>
@@ -5910,7 +6067,7 @@
       <c r="O71" s="7">
         <v>2</v>
       </c>
-      <c r="X71" s="20"/>
+      <c r="X71" s="19"/>
       <c r="AA71" s="7" t="s">
         <v>109</v>
       </c>
@@ -5932,18 +6089,18 @@
     </row>
     <row r="72" spans="2:41" ht="12.75" hidden="1" customHeight="1">
       <c r="B72" s="7" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="M72" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="N72" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="N72" s="22" t="s">
         <v>110</v>
       </c>
       <c r="O72">
         <v>4</v>
       </c>
-      <c r="X72" s="20"/>
+      <c r="X72" s="19"/>
       <c r="AA72" s="7" t="s">
         <v>111</v>
       </c>
@@ -5953,17 +6110,17 @@
       </c>
     </row>
     <row r="73" spans="2:41" ht="12.75" customHeight="1">
-      <c r="X73" s="20"/>
+      <c r="X73" s="19"/>
     </row>
     <row r="74" spans="2:41" ht="12.75" customHeight="1">
       <c r="B74" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="X74" s="20"/>
+        <v>321</v>
+      </c>
+      <c r="X74" s="19"/>
     </row>
     <row r="75" spans="2:41" ht="12.75" customHeight="1">
       <c r="B75" s="8" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>112</v>
@@ -5995,17 +6152,17 @@
       <c r="U75" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="V75" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="W75" s="7">
-        <v>1</v>
-      </c>
-      <c r="X75" s="21" t="s">
-        <v>381</v>
+      <c r="V75" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="W75" s="33">
+        <v>1</v>
+      </c>
+      <c r="X75" s="34" t="s">
+        <v>374</v>
       </c>
       <c r="Y75" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA75" s="7" t="s">
         <v>112</v>
@@ -6018,8 +6175,8 @@
       </c>
     </row>
     <row r="76" spans="2:41" ht="12.75" customHeight="1">
-      <c r="B76" s="7" t="s">
-        <v>325</v>
+      <c r="B76" s="21" t="s">
+        <v>443</v>
       </c>
       <c r="E76" s="7" t="s">
         <v>114</v>
@@ -6051,17 +6208,17 @@
       <c r="U76" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="V76" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="W76" s="7">
-        <v>1</v>
-      </c>
-      <c r="X76" s="21" t="s">
-        <v>380</v>
+      <c r="V76" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="W76" s="33">
+        <v>1</v>
+      </c>
+      <c r="X76" s="34" t="s">
+        <v>373</v>
       </c>
       <c r="Y76" s="8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AA76" s="7" t="s">
         <v>114</v>
@@ -6075,7 +6232,7 @@
     </row>
     <row r="77" spans="2:41" ht="12.75" customHeight="1">
       <c r="B77" s="7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E77" s="7" t="s">
         <v>116</v>
@@ -6104,11 +6261,11 @@
       <c r="W77" s="7">
         <v>1</v>
       </c>
-      <c r="X77" s="21" t="s">
-        <v>382</v>
+      <c r="X77" s="20" t="s">
+        <v>375</v>
       </c>
       <c r="Y77" s="8" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="AA77" s="7" t="s">
         <v>116</v>
@@ -6122,7 +6279,7 @@
     </row>
     <row r="78" spans="2:41" ht="12.75" customHeight="1">
       <c r="B78" s="7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>117</v>
@@ -6133,11 +6290,11 @@
       <c r="G78" s="7">
         <v>1</v>
       </c>
-      <c r="X78" s="20"/>
+      <c r="X78" s="19"/>
     </row>
     <row r="79" spans="2:41" ht="12.75" customHeight="1">
       <c r="B79" s="7" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>118</v>
@@ -6148,11 +6305,11 @@
       <c r="G79" s="7">
         <v>1</v>
       </c>
-      <c r="X79" s="20"/>
+      <c r="X79" s="19"/>
     </row>
     <row r="80" spans="2:41" ht="12.75" customHeight="1">
       <c r="B80" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>119</v>
@@ -6181,25 +6338,25 @@
       <c r="S80" s="7">
         <v>1</v>
       </c>
-      <c r="U80" s="19" t="s">
+      <c r="U80" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="V80" s="7" t="s">
+      <c r="V80" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="W80" s="7">
-        <v>1</v>
-      </c>
-      <c r="X80" s="21" t="s">
-        <v>383</v>
-      </c>
-      <c r="Y80" s="23" t="s">
-        <v>360</v>
+      <c r="W80" s="47">
+        <v>1</v>
+      </c>
+      <c r="X80" s="45" t="s">
+        <v>376</v>
+      </c>
+      <c r="Y80" s="47" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="81" spans="2:38" ht="12.75" customHeight="1">
       <c r="B81" s="7" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>122</v>
@@ -6219,7 +6376,7 @@
       <c r="O81" s="7">
         <v>2</v>
       </c>
-      <c r="X81" s="20"/>
+      <c r="X81" s="19"/>
       <c r="AA81" s="7" t="s">
         <v>122</v>
       </c>
@@ -6232,7 +6389,7 @@
     </row>
     <row r="82" spans="2:38" ht="12.75" customHeight="1">
       <c r="B82" s="7" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>124</v>
@@ -6243,11 +6400,11 @@
       <c r="G82" s="7">
         <v>1</v>
       </c>
-      <c r="X82" s="20"/>
+      <c r="X82" s="19"/>
     </row>
     <row r="83" spans="2:38" ht="12.75" customHeight="1">
       <c r="B83" s="7" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I83" s="7" t="s">
         <v>125</v>
@@ -6276,11 +6433,11 @@
       <c r="W83" s="7">
         <v>1</v>
       </c>
-      <c r="X83" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="Y83" s="22" t="s">
-        <v>371</v>
+      <c r="X83" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="Y83" s="21" t="s">
+        <v>365</v>
       </c>
       <c r="AA83" s="7" t="s">
         <v>125</v>
@@ -6294,7 +6451,7 @@
     </row>
     <row r="84" spans="2:38" ht="12.75" customHeight="1">
       <c r="B84" s="7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="M84" s="7" t="s">
         <v>126</v>
@@ -6305,11 +6462,11 @@
       <c r="O84" s="7">
         <v>2</v>
       </c>
-      <c r="X84" s="20"/>
+      <c r="X84" s="19"/>
     </row>
     <row r="85" spans="2:38" ht="12.75" customHeight="1">
       <c r="B85" s="7" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="M85" s="7" t="s">
         <v>127</v>
@@ -6320,11 +6477,11 @@
       <c r="O85" s="7">
         <v>1</v>
       </c>
-      <c r="X85" s="20"/>
+      <c r="X85" s="19"/>
     </row>
     <row r="86" spans="2:38" ht="12.75" customHeight="1">
       <c r="B86" s="7" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="M86" s="7" t="s">
         <v>129</v>
@@ -6335,7 +6492,7 @@
       <c r="O86" s="7">
         <v>1</v>
       </c>
-      <c r="X86" s="20"/>
+      <c r="X86" s="19"/>
       <c r="AA86" s="7" t="s">
         <v>129</v>
       </c>
@@ -6348,7 +6505,7 @@
     </row>
     <row r="87" spans="2:38" ht="12.75" customHeight="1">
       <c r="B87" s="7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="M87" s="7" t="s">
         <v>131</v>
@@ -6359,7 +6516,7 @@
       <c r="O87" s="7">
         <v>1</v>
       </c>
-      <c r="X87" s="20"/>
+      <c r="X87" s="19"/>
       <c r="AA87" s="7" t="s">
         <v>131</v>
       </c>
@@ -6371,17 +6528,17 @@
       </c>
     </row>
     <row r="88" spans="2:38" ht="12.75" customHeight="1">
-      <c r="X88" s="20"/>
+      <c r="X88" s="19"/>
     </row>
     <row r="89" spans="2:38" ht="12.75" customHeight="1">
       <c r="B89" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="X89" s="20"/>
+        <v>333</v>
+      </c>
+      <c r="X89" s="19"/>
     </row>
     <row r="90" spans="2:38" ht="12.75" customHeight="1">
       <c r="B90" s="7" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>132</v>
@@ -6428,7 +6585,7 @@
       <c r="W90" s="7">
         <v>1</v>
       </c>
-      <c r="X90" s="21"/>
+      <c r="X90" s="20"/>
       <c r="Y90" s="7"/>
       <c r="AA90" s="7" t="s">
         <v>132</v>
@@ -6442,7 +6599,7 @@
     </row>
     <row r="91" spans="2:38" ht="12.75" customHeight="1">
       <c r="B91" s="7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>134</v>
@@ -6479,7 +6636,7 @@
       <c r="W91" s="7">
         <v>22</v>
       </c>
-      <c r="X91" s="21"/>
+      <c r="X91" s="20"/>
       <c r="Y91" s="7"/>
       <c r="AA91" s="7" t="s">
         <v>134</v>
@@ -6498,7 +6655,7 @@
     </row>
     <row r="92" spans="2:38" ht="12.75" customHeight="1">
       <c r="B92" s="7" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>135</v>
@@ -6514,7 +6671,7 @@
       <c r="W92" s="7">
         <v>22</v>
       </c>
-      <c r="X92" s="21"/>
+      <c r="X92" s="20"/>
       <c r="Y92" s="7"/>
       <c r="AA92" s="7" t="s">
         <v>135</v>
@@ -6526,7 +6683,7 @@
     </row>
     <row r="93" spans="2:38" ht="12.75" customHeight="1">
       <c r="B93" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>136</v>
@@ -6535,11 +6692,11 @@
       <c r="G93" s="7">
         <v>22</v>
       </c>
-      <c r="X93" s="20"/>
+      <c r="X93" s="19"/>
     </row>
     <row r="94" spans="2:38" ht="12.75" customHeight="1">
       <c r="B94" s="7" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>86</v>
@@ -6586,7 +6743,7 @@
       <c r="W94" s="7">
         <v>2</v>
       </c>
-      <c r="X94" s="21"/>
+      <c r="X94" s="20"/>
       <c r="Y94" s="7"/>
       <c r="AA94" s="7" t="s">
         <v>86</v>
@@ -6600,7 +6757,7 @@
     </row>
     <row r="95" spans="2:38" ht="12.75" customHeight="1">
       <c r="B95" s="7" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="I95" s="7" t="s">
         <v>138</v>
@@ -6629,7 +6786,7 @@
       <c r="W95" s="7">
         <v>2</v>
       </c>
-      <c r="X95" s="21"/>
+      <c r="X95" s="20"/>
       <c r="Y95" s="7"/>
       <c r="AA95" s="7" t="s">
         <v>138</v>
@@ -6642,17 +6799,17 @@
       </c>
     </row>
     <row r="96" spans="2:38" ht="12.75" hidden="1" customHeight="1">
-      <c r="X96" s="20"/>
-    </row>
-    <row r="97" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+      <c r="X96" s="19"/>
+    </row>
+    <row r="97" spans="2:44" ht="12.75" hidden="1" customHeight="1">
       <c r="B97" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="X97" s="20"/>
-    </row>
-    <row r="98" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+        <v>340</v>
+      </c>
+      <c r="X97" s="19"/>
+    </row>
+    <row r="98" spans="2:44" ht="12.75" hidden="1" customHeight="1">
       <c r="B98" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="I98" s="7" t="s">
         <v>139</v>
@@ -6681,7 +6838,7 @@
       <c r="W98" s="7">
         <v>2</v>
       </c>
-      <c r="X98" s="21"/>
+      <c r="X98" s="20"/>
       <c r="Y98" s="7"/>
       <c r="AA98" s="7" t="s">
         <v>139</v>
@@ -6693,21 +6850,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="2:43" ht="12.75" hidden="1" customHeight="1">
-      <c r="X99" s="20"/>
-    </row>
-    <row r="100" spans="2:43" ht="12.75" customHeight="1">
-      <c r="X100" s="20"/>
-    </row>
-    <row r="101" spans="2:43" ht="24.75" customHeight="1">
-      <c r="B101" s="40" t="s">
-        <v>413</v>
-      </c>
-      <c r="X101" s="20"/>
-    </row>
-    <row r="102" spans="2:43" ht="12.75" customHeight="1">
+    <row r="99" spans="2:44" ht="12.75" hidden="1" customHeight="1">
+      <c r="X99" s="19"/>
+    </row>
+    <row r="100" spans="2:44" ht="12.75" customHeight="1">
+      <c r="X100" s="19"/>
+    </row>
+    <row r="101" spans="2:44" ht="24.75" customHeight="1">
+      <c r="B101" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="X101" s="19"/>
+    </row>
+    <row r="102" spans="2:44" ht="12.75" customHeight="1">
       <c r="B102" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>140</v>
@@ -6719,8 +6876,8 @@
       <c r="M102" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="N102" s="22" t="s">
-        <v>393</v>
+      <c r="N102" s="21" t="s">
+        <v>386</v>
       </c>
       <c r="O102" s="7">
         <v>1</v>
@@ -6732,20 +6889,20 @@
       <c r="S102" s="7">
         <v>1</v>
       </c>
-      <c r="U102" s="35" t="s">
+      <c r="U102" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="V102" s="39" t="s">
-        <v>407</v>
-      </c>
-      <c r="W102" s="35">
-        <v>1</v>
-      </c>
-      <c r="X102" s="36" t="s">
-        <v>408</v>
-      </c>
-      <c r="Y102" s="22" t="s">
-        <v>360</v>
+      <c r="V102" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="W102" s="33">
+        <v>1</v>
+      </c>
+      <c r="X102" s="34" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y102" s="21" t="s">
+        <v>354</v>
       </c>
       <c r="AA102" s="7" t="s">
         <v>140</v>
@@ -6761,10 +6918,13 @@
       <c r="AO102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="2:43" ht="12.75" customHeight="1">
-      <c r="B103" s="22" t="s">
-        <v>394</v>
+      <c r="AR102" s="22" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="103" spans="2:44" ht="12.75" customHeight="1">
+      <c r="B103" s="21" t="s">
+        <v>387</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>142</v>
@@ -6793,20 +6953,20 @@
       <c r="S103" s="7">
         <v>1</v>
       </c>
-      <c r="U103" s="37" t="s">
-        <v>409</v>
-      </c>
-      <c r="V103" s="35" t="s">
+      <c r="U103" s="35" t="s">
+        <v>402</v>
+      </c>
+      <c r="V103" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="W103" s="35">
-        <v>1</v>
-      </c>
-      <c r="X103" s="36" t="s">
-        <v>411</v>
-      </c>
-      <c r="Y103" s="22" t="s">
-        <v>360</v>
+      <c r="W103" s="33">
+        <v>1</v>
+      </c>
+      <c r="X103" s="34" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y103" s="21" t="s">
+        <v>354</v>
       </c>
       <c r="AA103" s="7" t="s">
         <v>142</v>
@@ -6818,9 +6978,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:43" ht="12.75" customHeight="1">
-      <c r="B104" s="22" t="s">
-        <v>395</v>
+    <row r="104" spans="2:44" ht="12.75" customHeight="1">
+      <c r="B104" s="21" t="s">
+        <v>388</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>143</v>
@@ -6849,20 +7009,20 @@
       <c r="S104" s="7">
         <v>1</v>
       </c>
-      <c r="U104" s="37" t="s">
-        <v>410</v>
-      </c>
-      <c r="V104" s="35" t="s">
+      <c r="U104" s="35" t="s">
+        <v>403</v>
+      </c>
+      <c r="V104" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="W104" s="35">
-        <v>1</v>
-      </c>
-      <c r="X104" s="36" t="s">
-        <v>412</v>
-      </c>
-      <c r="Y104" s="22" t="s">
-        <v>360</v>
+      <c r="W104" s="33">
+        <v>1</v>
+      </c>
+      <c r="X104" s="34" t="s">
+        <v>405</v>
+      </c>
+      <c r="Y104" s="21" t="s">
+        <v>354</v>
       </c>
       <c r="AA104" s="7" t="s">
         <v>143</v>
@@ -6874,9 +7034,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="2:43" ht="12.75" customHeight="1">
+    <row r="105" spans="2:44" ht="12.75" customHeight="1">
       <c r="B105" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E105" t="s">
         <v>144</v>
@@ -6885,10 +7045,10 @@
         <v>1</v>
       </c>
       <c r="M105" s="16" t="s">
-        <v>396</v>
-      </c>
-      <c r="N105" s="34" t="s">
-        <v>397</v>
+        <v>389</v>
+      </c>
+      <c r="N105" s="32" t="s">
+        <v>390</v>
       </c>
       <c r="Q105" t="s">
         <v>144</v>
@@ -6899,25 +7059,25 @@
       <c r="U105" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="V105" s="34" t="s">
-        <v>417</v>
-      </c>
-      <c r="W105" s="42">
-        <v>2</v>
-      </c>
-      <c r="X105" s="41" t="s">
-        <v>414</v>
-      </c>
-      <c r="Y105" s="24" t="s">
-        <v>360</v>
-      </c>
-      <c r="AQ105" s="34" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="106" spans="2:43" ht="12.75" customHeight="1">
+      <c r="V105" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="W105" s="40">
+        <v>2</v>
+      </c>
+      <c r="X105" s="39" t="s">
+        <v>407</v>
+      </c>
+      <c r="Y105" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="AQ105" s="32" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="106" spans="2:44" ht="12.75" customHeight="1">
       <c r="B106" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E106" s="7" t="s">
         <v>145</v>
@@ -6929,10 +7089,10 @@
         <v>1</v>
       </c>
       <c r="M106" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="N106" s="34" t="s">
-        <v>399</v>
+        <v>391</v>
+      </c>
+      <c r="N106" s="32" t="s">
+        <v>392</v>
       </c>
       <c r="Q106" s="7" t="s">
         <v>145</v>
@@ -6946,25 +7106,25 @@
       <c r="U106" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="V106" s="34" t="s">
-        <v>417</v>
-      </c>
-      <c r="W106" s="35">
-        <v>2</v>
-      </c>
-      <c r="X106" s="36" t="s">
-        <v>415</v>
-      </c>
-      <c r="Y106" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="AQ106" s="24" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="107" spans="2:43" ht="12.75" customHeight="1">
+      <c r="V106" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="W106" s="33">
+        <v>2</v>
+      </c>
+      <c r="X106" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="Y106" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="AQ106" s="22" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="107" spans="2:44" ht="12.75" customHeight="1">
       <c r="B107" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>146</v>
@@ -6976,9 +7136,9 @@
         <v>1</v>
       </c>
       <c r="M107" s="16" t="s">
-        <v>400</v>
-      </c>
-      <c r="N107" s="34" t="s">
+        <v>393</v>
+      </c>
+      <c r="N107" s="32" t="s">
         <v>147</v>
       </c>
       <c r="O107">
@@ -6987,25 +7147,25 @@
       <c r="U107" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="V107" s="34" t="s">
-        <v>417</v>
-      </c>
-      <c r="W107" s="35">
-        <v>2</v>
-      </c>
-      <c r="X107" s="36" t="s">
-        <v>419</v>
-      </c>
-      <c r="Y107" s="22" t="s">
-        <v>360</v>
+      <c r="V107" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="W107" s="33">
+        <v>2</v>
+      </c>
+      <c r="X107" s="34" t="s">
+        <v>412</v>
+      </c>
+      <c r="Y107" s="21" t="s">
+        <v>354</v>
       </c>
       <c r="AQ107" s="7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="108" spans="2:43" ht="12.75" customHeight="1">
-      <c r="B108" s="24" t="s">
-        <v>401</v>
+    <row r="108" spans="2:44" ht="12.75" customHeight="1">
+      <c r="B108" s="22" t="s">
+        <v>394</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>148</v>
@@ -7019,32 +7179,32 @@
       <c r="M108" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="N108" s="24" t="s">
+      <c r="N108" s="22" t="s">
         <v>147</v>
       </c>
       <c r="O108">
         <v>2</v>
       </c>
-      <c r="U108" s="35" t="s">
+      <c r="U108" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="V108" s="34" t="s">
-        <v>417</v>
-      </c>
-      <c r="W108" s="35">
-        <v>2</v>
-      </c>
-      <c r="X108" s="36" t="s">
-        <v>420</v>
+      <c r="V108" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="W108" s="33">
+        <v>2</v>
+      </c>
+      <c r="X108" s="34" t="s">
+        <v>413</v>
       </c>
       <c r="Y108" s="7"/>
       <c r="AQ108" s="7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="109" spans="2:43" ht="12.75" customHeight="1">
+    <row r="109" spans="2:44" ht="12.75" customHeight="1">
       <c r="B109" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>149</v>
@@ -7055,54 +7215,54 @@
       <c r="G109" s="7">
         <v>1</v>
       </c>
-      <c r="U109" s="35"/>
-      <c r="V109" s="43"/>
-      <c r="W109" s="35"/>
-      <c r="X109" s="36"/>
-      <c r="Y109" s="22"/>
+      <c r="U109" s="33"/>
+      <c r="V109" s="41"/>
+      <c r="W109" s="33"/>
+      <c r="X109" s="34"/>
+      <c r="Y109" s="21"/>
       <c r="AM109" s="7"/>
       <c r="AN109" s="7"/>
       <c r="AO109" s="7"/>
       <c r="AQ109" s="7"/>
     </row>
-    <row r="110" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B110" s="24" t="s">
-        <v>421</v>
+    <row r="110" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B110" s="22" t="s">
+        <v>455</v>
       </c>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
-      <c r="U110" s="35" t="s">
-        <v>422</v>
-      </c>
-      <c r="V110" s="43" t="s">
-        <v>417</v>
-      </c>
-      <c r="W110" s="35">
-        <v>2</v>
-      </c>
-      <c r="X110" s="36" t="s">
-        <v>423</v>
-      </c>
-      <c r="Y110" s="22"/>
+      <c r="U110" s="33" t="s">
+        <v>414</v>
+      </c>
+      <c r="V110" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="W110" s="33">
+        <v>2</v>
+      </c>
+      <c r="X110" s="34" t="s">
+        <v>415</v>
+      </c>
+      <c r="Y110" s="21"/>
       <c r="AM110" s="7"/>
       <c r="AN110" s="7"/>
       <c r="AO110" s="7"/>
-      <c r="AQ110" s="22" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="111" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+      <c r="AQ110" s="21" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="111" spans="2:44" ht="12.75" hidden="1" customHeight="1">
       <c r="B111" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="X111" s="20"/>
-    </row>
-    <row r="112" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+        <v>348</v>
+      </c>
+      <c r="X111" s="19"/>
+    </row>
+    <row r="112" spans="2:44" ht="12.75" hidden="1" customHeight="1">
       <c r="B112" t="s">
-        <v>349</v>
-      </c>
-      <c r="X112" s="20"/>
+        <v>345</v>
+      </c>
+      <c r="X112" s="19"/>
       <c r="AI112" t="s">
         <v>150</v>
       </c>
@@ -7113,11 +7273,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+    <row r="113" spans="2:44" ht="12.75" hidden="1" customHeight="1">
       <c r="B113" t="s">
-        <v>350</v>
-      </c>
-      <c r="X113" s="20"/>
+        <v>346</v>
+      </c>
+      <c r="X113" s="19"/>
       <c r="AI113" t="s">
         <v>151</v>
       </c>
@@ -7128,11 +7288,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+    <row r="114" spans="2:44" ht="12.75" hidden="1" customHeight="1">
       <c r="B114" t="s">
-        <v>353</v>
-      </c>
-      <c r="X114" s="20"/>
+        <v>349</v>
+      </c>
+      <c r="X114" s="19"/>
       <c r="AI114" t="s">
         <v>152</v>
       </c>
@@ -7143,11 +7303,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+    <row r="115" spans="2:44" ht="12.75" hidden="1" customHeight="1">
       <c r="B115" t="s">
-        <v>347</v>
-      </c>
-      <c r="X115" s="20"/>
+        <v>343</v>
+      </c>
+      <c r="X115" s="19"/>
       <c r="AI115" t="s">
         <v>153</v>
       </c>
@@ -7158,11 +7318,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="2:43" ht="12.75" hidden="1" customHeight="1">
+    <row r="116" spans="2:44" ht="12.75" hidden="1" customHeight="1">
       <c r="B116" t="s">
-        <v>348</v>
-      </c>
-      <c r="X116" s="20"/>
+        <v>344</v>
+      </c>
+      <c r="X116" s="19"/>
       <c r="AI116" t="s">
         <v>154</v>
       </c>
@@ -7173,18 +7333,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="2:43" ht="12.75" customHeight="1">
-      <c r="X117" s="20"/>
-    </row>
-    <row r="118" spans="2:43" ht="12.75" customHeight="1">
-      <c r="B118" s="44" t="s">
-        <v>428</v>
-      </c>
-      <c r="X118" s="20"/>
-    </row>
-    <row r="119" spans="2:43" ht="12.75" customHeight="1">
-      <c r="B119" s="22" t="s">
-        <v>425</v>
+    <row r="117" spans="2:44" ht="12.75" customHeight="1">
+      <c r="X117" s="19"/>
+    </row>
+    <row r="118" spans="2:44" ht="12.75" customHeight="1">
+      <c r="B118" s="42" t="s">
+        <v>420</v>
+      </c>
+      <c r="X118" s="19"/>
+    </row>
+    <row r="119" spans="2:44" ht="12.75" customHeight="1">
+      <c r="B119" s="21" t="s">
+        <v>417</v>
       </c>
       <c r="E119" s="7" t="s">
         <v>155</v>
@@ -7214,16 +7374,18 @@
       <c r="S119" s="7">
         <v>1</v>
       </c>
-      <c r="U119" s="37" t="s">
+      <c r="U119" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="V119" s="38" t="s">
+      <c r="V119" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="W119" s="7">
-        <v>1</v>
-      </c>
-      <c r="X119" s="21"/>
+      <c r="W119" s="33">
+        <v>1</v>
+      </c>
+      <c r="X119" s="34" t="s">
+        <v>427</v>
+      </c>
       <c r="Y119" s="7"/>
       <c r="AA119" s="7" t="s">
         <v>155</v>
@@ -7232,10 +7394,13 @@
       <c r="AC119" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="2:43" ht="12.75" customHeight="1">
-      <c r="B120" s="22" t="s">
-        <v>426</v>
+      <c r="AR119" s="22" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="120" spans="2:44" ht="12.75" customHeight="1">
+      <c r="B120" s="21" t="s">
+        <v>418</v>
       </c>
       <c r="E120" s="7" t="s">
         <v>156</v>
@@ -7255,16 +7420,18 @@
       <c r="S120" s="7">
         <v>4</v>
       </c>
-      <c r="U120" s="37" t="s">
+      <c r="U120" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="V120" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W120" s="7">
-        <v>2</v>
-      </c>
-      <c r="X120" s="21"/>
+      <c r="V120" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="W120" s="33">
+        <v>2</v>
+      </c>
+      <c r="X120" s="34" t="s">
+        <v>428</v>
+      </c>
       <c r="Y120" s="7"/>
       <c r="AA120" s="7" t="s">
         <v>156</v>
@@ -7275,13 +7442,13 @@
       <c r="AC120" s="7">
         <v>4</v>
       </c>
-      <c r="AQ120" s="24" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="121" spans="2:43" ht="12.75" customHeight="1">
-      <c r="B121" s="22" t="s">
-        <v>354</v>
+      <c r="AQ120" s="22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="121" spans="2:44" ht="12.75" customHeight="1">
+      <c r="B121" s="21" t="s">
+        <v>350</v>
       </c>
       <c r="E121" s="7" t="s">
         <v>157</v>
@@ -7304,16 +7471,18 @@
       <c r="S121" s="7">
         <v>1</v>
       </c>
-      <c r="U121" s="37" t="s">
+      <c r="U121" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="V121" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="W121" s="22" t="s">
-        <v>432</v>
-      </c>
-      <c r="X121" s="21"/>
+      <c r="V121" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="W121" s="35" t="s">
+        <v>424</v>
+      </c>
+      <c r="X121" s="34" t="s">
+        <v>429</v>
+      </c>
       <c r="Y121" s="7"/>
       <c r="AA121" s="7" t="s">
         <v>157</v>
@@ -7322,13 +7491,11 @@
       <c r="AC121" s="7">
         <v>1</v>
       </c>
-      <c r="AQ121" s="24" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="122" spans="2:43" ht="12.75" customHeight="1">
-      <c r="B122" s="22" t="s">
-        <v>427</v>
+      <c r="AQ121" s="22"/>
+    </row>
+    <row r="122" spans="2:44" ht="12.75" customHeight="1">
+      <c r="B122" s="21" t="s">
+        <v>419</v>
       </c>
       <c r="E122" s="7" t="s">
         <v>158</v>
@@ -7344,14 +7511,18 @@
       <c r="S122" s="7">
         <v>1</v>
       </c>
-      <c r="U122" s="37" t="s">
+      <c r="U122" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="V122" s="7"/>
-      <c r="W122" s="7">
-        <v>2</v>
-      </c>
-      <c r="X122" s="21"/>
+      <c r="V122" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="W122" s="33">
+        <v>2</v>
+      </c>
+      <c r="X122" s="34" t="s">
+        <v>430</v>
+      </c>
       <c r="Y122" s="7"/>
       <c r="AA122" s="7" t="s">
         <v>158</v>
@@ -7360,16 +7531,19 @@
       <c r="AC122" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B123" s="44" t="s">
-        <v>429</v>
-      </c>
-      <c r="X123" s="20"/>
-    </row>
-    <row r="124" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B124" s="22" t="s">
-        <v>425</v>
+      <c r="AQ122" s="22" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="123" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B123" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="X123" s="19"/>
+    </row>
+    <row r="124" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B124" s="21" t="s">
+        <v>417</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>155</v>
@@ -7399,14 +7573,18 @@
       <c r="S124" s="7">
         <v>1</v>
       </c>
-      <c r="U124" s="37" t="s">
+      <c r="U124" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="V124" s="7"/>
-      <c r="W124" s="7">
-        <v>1</v>
-      </c>
-      <c r="X124" s="21"/>
+      <c r="V124" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="W124" s="33">
+        <v>1</v>
+      </c>
+      <c r="X124" s="34" t="s">
+        <v>431</v>
+      </c>
       <c r="Y124" s="7"/>
       <c r="AA124" s="7" t="s">
         <v>155</v>
@@ -7416,9 +7594,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B125" s="22" t="s">
-        <v>426</v>
+    <row r="125" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B125" s="21" t="s">
+        <v>418</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>156</v>
@@ -7438,16 +7616,18 @@
       <c r="S125" s="7">
         <v>4</v>
       </c>
-      <c r="U125" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="V125" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W125" s="7">
-        <v>4</v>
-      </c>
-      <c r="X125" s="21"/>
+      <c r="U125" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="V125" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="W125" s="33">
+        <v>2</v>
+      </c>
+      <c r="X125" s="34" t="s">
+        <v>432</v>
+      </c>
       <c r="Y125" s="7"/>
       <c r="AA125" s="7" t="s">
         <v>156</v>
@@ -7458,10 +7638,13 @@
       <c r="AC125" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B126" s="22" t="s">
-        <v>354</v>
+      <c r="AQ125" s="22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="126" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B126" s="21" t="s">
+        <v>350</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>157</v>
@@ -7484,14 +7667,18 @@
       <c r="S126" s="7">
         <v>1</v>
       </c>
-      <c r="U126" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="V126" s="7"/>
-      <c r="W126" s="7">
-        <v>1</v>
-      </c>
-      <c r="X126" s="21"/>
+      <c r="U126" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="V126" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="W126" s="35" t="s">
+        <v>424</v>
+      </c>
+      <c r="X126" s="34" t="s">
+        <v>433</v>
+      </c>
       <c r="Y126" s="7"/>
       <c r="AA126" s="7" t="s">
         <v>157</v>
@@ -7500,10 +7687,11 @@
       <c r="AC126" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B127" s="22" t="s">
-        <v>427</v>
+      <c r="AQ126" s="22"/>
+    </row>
+    <row r="127" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B127" s="21" t="s">
+        <v>419</v>
       </c>
       <c r="E127" s="7" t="s">
         <v>158</v>
@@ -7519,14 +7707,18 @@
       <c r="S127" s="7">
         <v>1</v>
       </c>
-      <c r="U127" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="V127" s="7"/>
-      <c r="W127" s="7">
-        <v>1</v>
-      </c>
-      <c r="X127" s="21"/>
+      <c r="U127" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="V127" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="W127" s="33">
+        <v>2</v>
+      </c>
+      <c r="X127" s="34" t="s">
+        <v>434</v>
+      </c>
       <c r="Y127" s="7"/>
       <c r="AA127" s="7" t="s">
         <v>158</v>
@@ -7535,16 +7727,19 @@
       <c r="AC127" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B128" s="44" t="s">
-        <v>430</v>
-      </c>
-      <c r="X128" s="20"/>
-    </row>
-    <row r="129" spans="2:37" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B129" s="22" t="s">
-        <v>425</v>
+      <c r="AQ127" s="22" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="128" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B128" s="42" t="s">
+        <v>422</v>
+      </c>
+      <c r="X128" s="19"/>
+    </row>
+    <row r="129" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B129" s="21" t="s">
+        <v>417</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>155</v>
@@ -7574,14 +7769,18 @@
       <c r="S129" s="7">
         <v>1</v>
       </c>
-      <c r="U129" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="V129" s="7"/>
-      <c r="W129" s="7">
-        <v>1</v>
-      </c>
-      <c r="X129" s="21"/>
+      <c r="U129" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="V129" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="W129" s="33">
+        <v>1</v>
+      </c>
+      <c r="X129" s="34" t="s">
+        <v>435</v>
+      </c>
       <c r="Y129" s="7"/>
       <c r="AA129" s="7" t="s">
         <v>155</v>
@@ -7591,9 +7790,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:37" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B130" s="22" t="s">
-        <v>426</v>
+    <row r="130" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B130" s="21" t="s">
+        <v>418</v>
       </c>
       <c r="E130" s="7" t="s">
         <v>156</v>
@@ -7613,16 +7812,18 @@
       <c r="S130" s="7">
         <v>4</v>
       </c>
-      <c r="U130" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="V130" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W130" s="7">
-        <v>4</v>
-      </c>
-      <c r="X130" s="21"/>
+      <c r="U130" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="V130" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="W130" s="33">
+        <v>2</v>
+      </c>
+      <c r="X130" s="34" t="s">
+        <v>436</v>
+      </c>
       <c r="Y130" s="7"/>
       <c r="AA130" s="7" t="s">
         <v>156</v>
@@ -7633,10 +7834,13 @@
       <c r="AC130" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="131" spans="2:37" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B131" s="22" t="s">
-        <v>354</v>
+      <c r="AQ130" s="22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="131" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B131" s="21" t="s">
+        <v>350</v>
       </c>
       <c r="E131" s="7" t="s">
         <v>157</v>
@@ -7659,14 +7863,18 @@
       <c r="S131" s="7">
         <v>1</v>
       </c>
-      <c r="U131" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="V131" s="7"/>
-      <c r="W131" s="7">
-        <v>1</v>
-      </c>
-      <c r="X131" s="21"/>
+      <c r="U131" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="V131" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="W131" s="35" t="s">
+        <v>424</v>
+      </c>
+      <c r="X131" s="34" t="s">
+        <v>437</v>
+      </c>
       <c r="Y131" s="7"/>
       <c r="AA131" s="7" t="s">
         <v>157</v>
@@ -7675,10 +7883,11 @@
       <c r="AC131" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="2:37" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B132" s="22" t="s">
-        <v>427</v>
+      <c r="AQ131" s="22"/>
+    </row>
+    <row r="132" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B132" s="21" t="s">
+        <v>419</v>
       </c>
       <c r="E132" s="7" t="s">
         <v>158</v>
@@ -7694,14 +7903,18 @@
       <c r="S132" s="7">
         <v>1</v>
       </c>
-      <c r="U132" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="V132" s="7"/>
-      <c r="W132" s="7">
-        <v>1</v>
-      </c>
-      <c r="X132" s="21"/>
+      <c r="U132" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="V132" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="W132" s="33">
+        <v>2</v>
+      </c>
+      <c r="X132" s="34" t="s">
+        <v>438</v>
+      </c>
       <c r="Y132" s="7"/>
       <c r="AA132" s="7" t="s">
         <v>158</v>
@@ -7710,252 +7923,255 @@
       <c r="AC132" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="2:37" ht="12.75" customHeight="1">
-      <c r="B133" s="7"/>
-      <c r="E133" s="7" t="s">
-        <v>159</v>
-      </c>
+      <c r="AQ132" s="22" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="133" spans="2:43" s="16" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B133" s="21"/>
+      <c r="E133" s="7"/>
       <c r="F133" s="7"/>
-      <c r="G133" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q133" s="7" t="s">
-        <v>159</v>
-      </c>
+      <c r="G133" s="7"/>
+      <c r="Q133" s="7"/>
       <c r="R133" s="7"/>
-      <c r="S133" s="7">
-        <v>1</v>
-      </c>
-      <c r="U133" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="V133" s="7"/>
-      <c r="W133" s="7">
-        <v>1</v>
-      </c>
-      <c r="X133" s="21"/>
+      <c r="S133" s="7"/>
       <c r="Y133" s="7"/>
-      <c r="AA133" s="7" t="s">
-        <v>159</v>
-      </c>
+      <c r="AA133" s="7"/>
       <c r="AB133" s="7"/>
-      <c r="AC133" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="2:37" ht="12.75" customHeight="1">
+      <c r="AC133" s="7"/>
+      <c r="AQ133" s="22"/>
+    </row>
+    <row r="134" spans="2:43" ht="12.75" customHeight="1">
       <c r="B134" s="7"/>
       <c r="E134" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F134" s="7" t="s">
-        <v>23</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="F134" s="7"/>
       <c r="G134" s="7">
-        <v>2</v>
-      </c>
-      <c r="M134" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="N134" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O134" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q134" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="R134" s="7" t="s">
-        <v>23</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="R134" s="7"/>
       <c r="S134" s="7">
-        <v>2</v>
-      </c>
-      <c r="U134" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="V134" s="7" t="s">
-        <v>23</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="U134" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="V134" s="7"/>
       <c r="W134" s="7">
-        <v>2</v>
-      </c>
-      <c r="X134" s="21"/>
+        <v>1</v>
+      </c>
+      <c r="X134" s="20"/>
       <c r="Y134" s="7"/>
       <c r="AA134" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AB134" s="7" t="s">
-        <v>23</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="AB134" s="7"/>
       <c r="AC134" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="135" spans="2:37" ht="12.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:43" ht="12.75" customHeight="1">
       <c r="B135" s="7"/>
       <c r="E135" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G135" s="7">
+        <v>2</v>
+      </c>
+      <c r="M135" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="N135" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O135" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q135" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="R135" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S135" s="7">
+        <v>2</v>
+      </c>
+      <c r="U135" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="V135" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="W135" s="7">
+        <v>2</v>
+      </c>
+      <c r="X135" s="20"/>
+      <c r="Y135" s="7"/>
+      <c r="AA135" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB135" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC135" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="2:43" ht="12.75" customHeight="1">
+      <c r="B136" s="7"/>
+      <c r="E136" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="G135" s="7">
-        <v>1</v>
-      </c>
-      <c r="M135" s="7" t="s">
+      <c r="G136" s="7">
+        <v>1</v>
+      </c>
+      <c r="M136" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="O135" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q135" s="7" t="s">
+      <c r="O136" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q136" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="S135" s="7">
-        <v>1</v>
-      </c>
-      <c r="U135" s="17" t="s">
+      <c r="S136" s="7">
+        <v>1</v>
+      </c>
+      <c r="U136" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="W135" s="7">
-        <v>1</v>
-      </c>
-      <c r="X135" s="21" t="s">
-        <v>385</v>
-      </c>
-      <c r="Y135" s="22" t="s">
-        <v>371</v>
-      </c>
-      <c r="AA135" s="7" t="s">
+      <c r="W136" s="7">
+        <v>1</v>
+      </c>
+      <c r="X136" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="Y136" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="AA136" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="AC135" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="2:37">
-      <c r="B137" s="2" t="s">
+      <c r="AC136" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="2:43">
+      <c r="B138" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="2:37" ht="25.5">
-      <c r="B138" s="7" t="s">
+    <row r="139" spans="2:43" ht="25.5">
+      <c r="B139" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="AI138" t="s">
+      <c r="AI139" t="s">
         <v>164</v>
       </c>
-      <c r="AJ138" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK138">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="2:37" ht="25.5">
-      <c r="B139" s="7" t="s">
+      <c r="AJ139" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="2:43" ht="25.5">
+      <c r="B140" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="AI139" t="s">
+      <c r="AI140" t="s">
         <v>166</v>
       </c>
-      <c r="AJ139" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK139">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="2:37" ht="25.5">
-      <c r="B140" s="7" t="s">
+      <c r="AJ140" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="2:43" ht="25.5">
+      <c r="B141" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="AI140" t="s">
+      <c r="AI141" t="s">
         <v>168</v>
       </c>
-      <c r="AJ140" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK140">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="141" spans="2:37" ht="25.5">
-      <c r="B141" s="7" t="s">
+      <c r="AJ141" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="2:43" ht="25.5">
+      <c r="B142" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="AI141" t="s">
+      <c r="AI142" t="s">
         <v>170</v>
       </c>
-      <c r="AJ141" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK141">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="142" spans="2:37" ht="25.5">
-      <c r="B142" s="7" t="s">
+      <c r="AJ142" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="2:43" ht="25.5">
+      <c r="B143" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="AI142" t="s">
+      <c r="AI143" t="s">
         <v>172</v>
       </c>
-      <c r="AJ142" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK142">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="143" spans="2:37" ht="25.5">
-      <c r="B143" s="7" t="s">
+      <c r="AJ143" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="2:43" ht="25.5">
+      <c r="B144" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="AI143" t="s">
+      <c r="AI144" t="s">
         <v>174</v>
       </c>
-      <c r="AJ143" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK143">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="144" spans="2:37" ht="25.5">
-      <c r="B144" t="s">
+      <c r="AJ144" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="2:37" ht="25.5">
+      <c r="B145" t="s">
         <v>175</v>
       </c>
-      <c r="AI144" t="s">
+      <c r="AI145" t="s">
         <v>176</v>
       </c>
-      <c r="AJ144" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK144">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="145" spans="2:37" ht="25.5">
-      <c r="B145" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="AI145" t="s">
-        <v>178</v>
-      </c>
-      <c r="AJ145" s="7" t="s">
-        <v>95</v>
+      <c r="AJ145" t="s">
+        <v>23</v>
       </c>
       <c r="AK145">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="2:37" ht="25.5">
       <c r="B146" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AI146" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AJ146" s="7" t="s">
         <v>95</v>
@@ -7966,10 +8182,10 @@
     </row>
     <row r="147" spans="2:37" ht="25.5">
       <c r="B147" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AI147" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AJ147" s="7" t="s">
         <v>95</v>
@@ -7980,10 +8196,10 @@
     </row>
     <row r="148" spans="2:37" ht="25.5">
       <c r="B148" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AI148" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AJ148" s="7" t="s">
         <v>95</v>
@@ -7994,10 +8210,10 @@
     </row>
     <row r="149" spans="2:37" ht="25.5">
       <c r="B149" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AI149" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AJ149" s="7" t="s">
         <v>95</v>
@@ -8008,10 +8224,10 @@
     </row>
     <row r="150" spans="2:37" ht="25.5">
       <c r="B150" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AI150" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AJ150" s="7" t="s">
         <v>95</v>
@@ -8022,10 +8238,10 @@
     </row>
     <row r="151" spans="2:37" ht="25.5">
       <c r="B151" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AI151" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AJ151" s="7" t="s">
         <v>95</v>
@@ -8036,10 +8252,10 @@
     </row>
     <row r="152" spans="2:37" ht="25.5">
       <c r="B152" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AI152" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AJ152" s="7" t="s">
         <v>95</v>
@@ -8050,10 +8266,10 @@
     </row>
     <row r="153" spans="2:37" ht="25.5">
       <c r="B153" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AI153" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AJ153" s="7" t="s">
         <v>95</v>
@@ -8064,10 +8280,10 @@
     </row>
     <row r="154" spans="2:37" ht="25.5">
       <c r="B154" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AI154" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AJ154" s="7" t="s">
         <v>95</v>
@@ -8078,10 +8294,10 @@
     </row>
     <row r="155" spans="2:37" ht="25.5">
       <c r="B155" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AI155" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AJ155" s="7" t="s">
         <v>95</v>
@@ -8092,10 +8308,10 @@
     </row>
     <row r="156" spans="2:37" ht="25.5">
       <c r="B156" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AI156" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AJ156" s="7" t="s">
         <v>95</v>
@@ -8106,10 +8322,13 @@
     </row>
     <row r="157" spans="2:37" ht="25.5">
       <c r="B157" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AI157" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="AJ157" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="AK157">
         <v>4</v>
@@ -8117,10 +8336,10 @@
     </row>
     <row r="158" spans="2:37" ht="25.5">
       <c r="B158" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AI158" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AK158">
         <v>4</v>
@@ -8128,10 +8347,10 @@
     </row>
     <row r="159" spans="2:37" ht="25.5">
       <c r="B159" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AI159" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="AK159">
         <v>4</v>
@@ -8139,10 +8358,10 @@
     </row>
     <row r="160" spans="2:37" ht="25.5">
       <c r="B160" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AI160" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AK160">
         <v>4</v>
@@ -8150,10 +8369,10 @@
     </row>
     <row r="161" spans="2:37" ht="25.5">
       <c r="B161" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AI161" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="AK161">
         <v>4</v>
@@ -8161,10 +8380,10 @@
     </row>
     <row r="162" spans="2:37" ht="25.5">
       <c r="B162" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="AI162" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AK162">
         <v>4</v>
@@ -8172,10 +8391,10 @@
     </row>
     <row r="163" spans="2:37" ht="25.5">
       <c r="B163" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AI163" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AK163">
         <v>4</v>
@@ -8183,10 +8402,10 @@
     </row>
     <row r="164" spans="2:37" ht="25.5">
       <c r="B164" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AI164" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="AK164">
         <v>4</v>
@@ -8194,10 +8413,10 @@
     </row>
     <row r="165" spans="2:37" ht="25.5">
       <c r="B165" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AI165" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AK165">
         <v>4</v>
@@ -8205,10 +8424,10 @@
     </row>
     <row r="166" spans="2:37" ht="25.5">
       <c r="B166" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AI166" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AK166">
         <v>4</v>
@@ -8216,10 +8435,10 @@
     </row>
     <row r="167" spans="2:37" ht="25.5">
       <c r="B167" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AI167" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AK167">
         <v>4</v>
@@ -8227,10 +8446,10 @@
     </row>
     <row r="168" spans="2:37" ht="25.5">
       <c r="B168" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AI168" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK168">
         <v>4</v>
@@ -8238,24 +8457,21 @@
     </row>
     <row r="169" spans="2:37" ht="25.5">
       <c r="B169" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI169" t="s">
+        <v>224</v>
+      </c>
+      <c r="AK169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="2:37" ht="25.5">
+      <c r="B170" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="AI169" t="s">
+      <c r="AI170" t="s">
         <v>226</v>
-      </c>
-      <c r="AJ169" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="2:37" ht="25.5">
-      <c r="B170" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI170" t="s">
-        <v>228</v>
       </c>
       <c r="AJ170" t="s">
         <v>88</v>
@@ -8266,10 +8482,10 @@
     </row>
     <row r="171" spans="2:37" ht="25.5">
       <c r="B171" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AI171" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AJ171" t="s">
         <v>88</v>
@@ -8279,11 +8495,11 @@
       </c>
     </row>
     <row r="172" spans="2:37" ht="25.5">
-      <c r="B172" s="7" t="s">
-        <v>231</v>
+      <c r="B172" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="AI172" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AJ172" t="s">
         <v>88</v>
@@ -8294,10 +8510,10 @@
     </row>
     <row r="173" spans="2:37" ht="25.5">
       <c r="B173" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AI173" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AJ173" t="s">
         <v>88</v>
@@ -8308,10 +8524,10 @@
     </row>
     <row r="174" spans="2:37" ht="25.5">
       <c r="B174" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AI174" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AJ174" t="s">
         <v>88</v>
@@ -8322,10 +8538,10 @@
     </row>
     <row r="175" spans="2:37" ht="25.5">
       <c r="B175" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AI175" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AJ175" t="s">
         <v>88</v>
@@ -8336,10 +8552,10 @@
     </row>
     <row r="176" spans="2:37" ht="25.5">
       <c r="B176" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AI176" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AJ176" t="s">
         <v>88</v>
@@ -8350,10 +8566,10 @@
     </row>
     <row r="177" spans="2:41" ht="25.5">
       <c r="B177" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AI177" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AJ177" t="s">
         <v>88</v>
@@ -8364,10 +8580,10 @@
     </row>
     <row r="178" spans="2:41" ht="25.5">
       <c r="B178" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AI178" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AJ178" t="s">
         <v>88</v>
@@ -8378,10 +8594,10 @@
     </row>
     <row r="179" spans="2:41" ht="25.5">
       <c r="B179" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AI179" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="AJ179" t="s">
         <v>88</v>
@@ -8392,10 +8608,10 @@
     </row>
     <row r="180" spans="2:41" ht="25.5">
       <c r="B180" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AI180" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AJ180" t="s">
         <v>88</v>
@@ -8404,34 +8620,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="2:41">
-      <c r="B181" s="7"/>
+    <row r="181" spans="2:41" ht="25.5">
+      <c r="B181" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI181" t="s">
+        <v>248</v>
+      </c>
+      <c r="AJ181" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK181">
+        <v>1</v>
+      </c>
     </row>
     <row r="182" spans="2:41">
-      <c r="B182" s="2" t="s">
+      <c r="B182" s="7"/>
+    </row>
+    <row r="183" spans="2:41">
+      <c r="B183" s="2" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="183" spans="2:41" ht="25.5">
-      <c r="B183" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="AM183" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN183" t="s">
-        <v>23</v>
-      </c>
-      <c r="AO183">
-        <v>2</v>
       </c>
     </row>
     <row r="184" spans="2:41" ht="25.5">
       <c r="B184" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AM184" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AN184" t="s">
         <v>23</v>
@@ -8442,10 +8658,10 @@
     </row>
     <row r="185" spans="2:41" ht="25.5">
       <c r="B185" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AM185" t="s">
-        <v>253</v>
+        <v>59</v>
       </c>
       <c r="AN185" t="s">
         <v>23</v>
@@ -8456,10 +8672,10 @@
     </row>
     <row r="186" spans="2:41" ht="25.5">
       <c r="B186" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AM186" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AN186" t="s">
         <v>23</v>
@@ -8470,10 +8686,10 @@
     </row>
     <row r="187" spans="2:41" ht="25.5">
       <c r="B187" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AM187" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AN187" t="s">
         <v>23</v>
@@ -8484,10 +8700,10 @@
     </row>
     <row r="188" spans="2:41" ht="25.5">
       <c r="B188" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AM188" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AN188" t="s">
         <v>23</v>
@@ -8498,24 +8714,24 @@
     </row>
     <row r="189" spans="2:41" ht="25.5">
       <c r="B189" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AM189" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AN189" t="s">
-        <v>130</v>
+        <v>23</v>
       </c>
       <c r="AO189">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190" spans="2:41" ht="25.5">
       <c r="B190" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AM190" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AN190" t="s">
         <v>130</v>
@@ -8526,24 +8742,24 @@
     </row>
     <row r="191" spans="2:41" ht="25.5">
       <c r="B191" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AM191" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AN191" t="s">
-        <v>266</v>
+        <v>130</v>
       </c>
       <c r="AO191">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="2:41" ht="25.5">
       <c r="B192" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="AM192" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="AN192" t="s">
         <v>266</v>
@@ -8554,31 +8770,42 @@
     </row>
     <row r="193" spans="2:41" ht="25.5">
       <c r="B193" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AM193" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AN193" t="s">
-        <v>130</v>
+        <v>266</v>
       </c>
       <c r="AO193">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="194" spans="2:41" ht="25.5">
       <c r="B194" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="AM194" t="s">
+        <v>270</v>
+      </c>
+      <c r="AN194" t="s">
+        <v>130</v>
+      </c>
+      <c r="AO194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="2:41" ht="25.5">
+      <c r="B195" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="AM194" t="s">
+      <c r="AM195" t="s">
         <v>272</v>
       </c>
-      <c r="AO194">
+      <c r="AO195">
         <v>4</v>
       </c>
-    </row>
-    <row r="195" spans="2:41">
-      <c r="B195" s="7"/>
     </row>
     <row r="196" spans="2:41">
       <c r="B196" s="7"/>
@@ -8631,8 +8858,11 @@
     <row r="212" spans="2:2">
       <c r="B212" s="7"/>
     </row>
-    <row r="5207" spans="7:23" ht="12.75" customHeight="1"/>
+    <row r="213" spans="2:2">
+      <c r="B213" s="7"/>
+    </row>
     <row r="5208" spans="7:23" ht="12.75" customHeight="1"/>
+    <row r="5209" spans="7:23" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="AA2:AC2"/>

</xml_diff>

<commit_message>
Updated vcontrold after modifying data types
</commit_message>
<xml_diff>
--- a/Optolink_Logger_v3.xlsx
+++ b/Optolink_Logger_v3.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\GitHub\Viessmann-Control\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="150" yWindow="510" windowWidth="25080" windowHeight="11445"/>
   </bookViews>
@@ -25,7 +20,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="V3" authorId="0" shapeId="0">
+    <comment ref="V3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -38,7 +33,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF3" authorId="0" shapeId="0">
+    <comment ref="AF3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN3" authorId="0" shapeId="0">
+    <comment ref="AN3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB11" authorId="0" shapeId="0">
+    <comment ref="AB11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N26" authorId="0" shapeId="0">
+    <comment ref="N26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N30" authorId="0" shapeId="0">
+    <comment ref="N30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB42" authorId="0" shapeId="0">
+    <comment ref="AB42" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC70" authorId="0" shapeId="0">
+    <comment ref="AC70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O78" authorId="0" shapeId="0">
+    <comment ref="O78" authorId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O79" authorId="0" shapeId="0">
+    <comment ref="O79" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O82" authorId="0" shapeId="0">
+    <comment ref="O82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O83" authorId="0" shapeId="0">
+    <comment ref="O83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G89" authorId="0" shapeId="0">
+    <comment ref="G89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K89" authorId="0" shapeId="0">
+    <comment ref="K89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O89" authorId="0" shapeId="0">
+    <comment ref="O89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -228,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S89" authorId="0" shapeId="0">
+    <comment ref="S89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W89" authorId="0" shapeId="0">
+    <comment ref="W89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -256,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC89" authorId="0" shapeId="0">
+    <comment ref="AC89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL89" authorId="0" shapeId="0">
+    <comment ref="AL89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G90" authorId="0" shapeId="0">
+    <comment ref="G90" authorId="0">
       <text>
         <r>
           <rPr>
@@ -298,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W90" authorId="0" shapeId="0">
+    <comment ref="W90" authorId="0">
       <text>
         <r>
           <rPr>
@@ -312,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC90" authorId="0" shapeId="0">
+    <comment ref="AC90" authorId="0">
       <text>
         <r>
           <rPr>
@@ -326,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G91" authorId="0" shapeId="0">
+    <comment ref="G91" authorId="0">
       <text>
         <r>
           <rPr>
@@ -340,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G92" authorId="0" shapeId="0">
+    <comment ref="G92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -353,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K92" authorId="0" shapeId="0">
+    <comment ref="K92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -366,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O92" authorId="0" shapeId="0">
+    <comment ref="O92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S92" authorId="0" shapeId="0">
+    <comment ref="S92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W92" authorId="0" shapeId="0">
+    <comment ref="W92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC92" authorId="0" shapeId="0">
+    <comment ref="AC92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -418,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K93" authorId="0" shapeId="0">
+    <comment ref="K93" authorId="0">
       <text>
         <r>
           <rPr>
@@ -431,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S93" authorId="0" shapeId="0">
+    <comment ref="S93" authorId="0">
       <text>
         <r>
           <rPr>
@@ -444,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W93" authorId="0" shapeId="0">
+    <comment ref="W93" authorId="0">
       <text>
         <r>
           <rPr>
@@ -457,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC93" authorId="0" shapeId="0">
+    <comment ref="AC93" authorId="0">
       <text>
         <r>
           <rPr>
@@ -470,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G100" authorId="0" shapeId="0">
+    <comment ref="G100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -487,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O100" authorId="0" shapeId="0">
+    <comment ref="O100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -503,7 +498,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S100" authorId="0" shapeId="0">
+    <comment ref="S100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -520,7 +515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W100" authorId="0" shapeId="0">
+    <comment ref="W100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -537,7 +532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC100" authorId="0" shapeId="0">
+    <comment ref="AC100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -554,7 +549,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO100" authorId="0" shapeId="0">
+    <comment ref="AO100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -569,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G114" authorId="0" shapeId="0">
+    <comment ref="G114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -585,7 +580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K114" authorId="0" shapeId="0">
+    <comment ref="K114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -601,7 +596,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O114" authorId="0" shapeId="0">
+    <comment ref="O114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -617,7 +612,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S114" authorId="0" shapeId="0">
+    <comment ref="S114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -633,7 +628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W114" authorId="0" shapeId="0">
+    <comment ref="W114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -649,7 +644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC114" authorId="0" shapeId="0">
+    <comment ref="AC114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -665,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G116" authorId="0" shapeId="0">
+    <comment ref="G116" authorId="0">
       <text>
         <r>
           <rPr>
@@ -679,7 +674,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K116" authorId="0" shapeId="0">
+    <comment ref="K116" authorId="0">
       <text>
         <r>
           <rPr>
@@ -693,7 +688,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S116" authorId="0" shapeId="0">
+    <comment ref="S116" authorId="0">
       <text>
         <r>
           <rPr>
@@ -707,7 +702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W116" authorId="0" shapeId="0">
+    <comment ref="W116" authorId="0">
       <text>
         <r>
           <rPr>
@@ -721,7 +716,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC116" authorId="0" shapeId="0">
+    <comment ref="AC116" authorId="0">
       <text>
         <r>
           <rPr>
@@ -735,7 +730,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G117" authorId="0" shapeId="0">
+    <comment ref="G117" authorId="0">
       <text>
         <r>
           <rPr>
@@ -750,7 +745,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S117" authorId="0" shapeId="0">
+    <comment ref="S117" authorId="0">
       <text>
         <r>
           <rPr>
@@ -765,7 +760,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W117" authorId="0" shapeId="0">
+    <comment ref="W117" authorId="0">
       <text>
         <r>
           <rPr>
@@ -780,7 +775,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC117" authorId="0" shapeId="0">
+    <comment ref="AC117" authorId="0">
       <text>
         <r>
           <rPr>
@@ -795,7 +790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G118" authorId="0" shapeId="0">
+    <comment ref="G118" authorId="0">
       <text>
         <r>
           <rPr>
@@ -808,7 +803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S118" authorId="0" shapeId="0">
+    <comment ref="S118" authorId="0">
       <text>
         <r>
           <rPr>
@@ -821,7 +816,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W118" authorId="0" shapeId="0">
+    <comment ref="W118" authorId="0">
       <text>
         <r>
           <rPr>
@@ -834,7 +829,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC118" authorId="0" shapeId="0">
+    <comment ref="AC118" authorId="0">
       <text>
         <r>
           <rPr>
@@ -847,7 +842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G123" authorId="0" shapeId="0">
+    <comment ref="G123" authorId="0">
       <text>
         <r>
           <rPr>
@@ -860,7 +855,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S123" authorId="0" shapeId="0">
+    <comment ref="S123" authorId="0">
       <text>
         <r>
           <rPr>
@@ -873,7 +868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W123" authorId="0" shapeId="0">
+    <comment ref="W123" authorId="0">
       <text>
         <r>
           <rPr>
@@ -886,7 +881,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC123" authorId="0" shapeId="0">
+    <comment ref="AC123" authorId="0">
       <text>
         <r>
           <rPr>
@@ -899,7 +894,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G128" authorId="0" shapeId="0">
+    <comment ref="G128" authorId="0">
       <text>
         <r>
           <rPr>
@@ -912,7 +907,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S128" authorId="0" shapeId="0">
+    <comment ref="S128" authorId="0">
       <text>
         <r>
           <rPr>
@@ -925,7 +920,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W128" authorId="0" shapeId="0">
+    <comment ref="W128" authorId="0">
       <text>
         <r>
           <rPr>
@@ -938,7 +933,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC128" authorId="0" shapeId="0">
+    <comment ref="AC128" authorId="0">
       <text>
         <r>
           <rPr>
@@ -951,7 +946,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5208" authorId="0" shapeId="0">
+    <comment ref="G5208" authorId="0">
       <text>
         <r>
           <rPr>
@@ -963,7 +958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S5208" authorId="0" shapeId="0">
+    <comment ref="S5208" authorId="0">
       <text>
         <r>
           <rPr>
@@ -975,7 +970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W5208" authorId="0" shapeId="0">
+    <comment ref="W5208" authorId="0">
       <text>
         <r>
           <rPr>
@@ -987,7 +982,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5209" authorId="0" shapeId="0">
+    <comment ref="G5209" authorId="0">
       <text>
         <r>
           <rPr>
@@ -999,7 +994,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S5209" authorId="0" shapeId="0">
+    <comment ref="S5209" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1011,7 +1006,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W5209" authorId="0" shapeId="0">
+    <comment ref="W5209" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1028,7 +1023,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="486">
   <si>
     <t>V333MW1</t>
   </si>
@@ -2425,16 +2420,89 @@
   </si>
   <si>
     <t>DT</t>
+  </si>
+  <si>
+    <t>works</t>
+  </si>
+  <si>
+    <t>Scaled</t>
+  </si>
+  <si>
+    <t>0x6600</t>
+  </si>
+  <si>
+    <t>0x2098</t>
+  </si>
+  <si>
+    <t>Raw value (hex)</t>
+  </si>
+  <si>
+    <t>0x8100</t>
+  </si>
+  <si>
+    <t>short - float</t>
+  </si>
+  <si>
+    <t>0xEC00</t>
+  </si>
+  <si>
+    <t>0xFFFF</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>0x6D00</t>
+  </si>
+  <si>
+    <t>0xED00</t>
+  </si>
+  <si>
+    <t>0xC800</t>
+  </si>
+  <si>
+    <t>0x7800</t>
+  </si>
+  <si>
+    <t>0xFF</t>
+  </si>
+  <si>
+    <t>0x00720000</t>
+  </si>
+  <si>
+    <t>0x4D119E00</t>
+  </si>
+  <si>
+    <t>2877.532471 hours</t>
+  </si>
+  <si>
+    <t>uint</t>
+  </si>
+  <si>
+    <t>0xB1083400</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>0x32FF</t>
+  </si>
+  <si>
+    <t>short float</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2648,7 +2716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2738,6 +2806,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2750,13 +2831,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2913,7 +2990,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2945,10 +3022,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2980,7 +3056,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3156,17 +3231,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AR5209"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:AV5209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="U24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="T76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="AV110" sqref="AV110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="0.7109375" customWidth="1"/>
     <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
@@ -3213,7 +3288,7 @@
     <col min="43" max="43" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:48" ht="18" customHeight="1">
       <c r="B1" s="10" t="s">
         <v>280</v>
       </c>
@@ -3257,54 +3332,54 @@
       <c r="AO1" s="15"/>
       <c r="AP1" s="15"/>
     </row>
-    <row r="2" spans="2:44" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E2" s="45" t="s">
+    <row r="2" spans="2:48" ht="21.75" customHeight="1">
+      <c r="E2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="I2" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="M2" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="Q2" s="45" t="s">
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="I2" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="M2" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="Q2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="U2" s="45" t="s">
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="U2" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="AA2" s="45" t="s">
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="AA2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AE2" s="47" t="s">
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AE2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="AF2" s="47"/>
-      <c r="AG2" s="47"/>
-      <c r="AI2" s="47" t="s">
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="52"/>
+      <c r="AI2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AM2" s="47" t="s">
+      <c r="AJ2" s="53"/>
+      <c r="AK2" s="53"/>
+      <c r="AM2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-    </row>
-    <row r="3" spans="2:44" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="53"/>
+    </row>
+    <row r="3" spans="2:48" ht="27.75" customHeight="1">
       <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3351,7 +3426,7 @@
         <v>11</v>
       </c>
       <c r="X3" s="12"/>
-      <c r="Y3" s="49" t="s">
+      <c r="Y3" s="47" t="s">
         <v>460</v>
       </c>
       <c r="AA3" s="9" t="s">
@@ -3398,8 +3473,17 @@
       <c r="AR3" s="22" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="4" spans="2:44" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS3" s="45" t="s">
+        <v>462</v>
+      </c>
+      <c r="AT3" s="46" t="s">
+        <v>466</v>
+      </c>
+      <c r="AU3" s="45" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="4" spans="2:48" ht="21.75" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>281</v>
       </c>
@@ -3487,19 +3571,28 @@
       <c r="AR4" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="5" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS4" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT4" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="AU4">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="5" spans="2:48" ht="12.75" customHeight="1">
       <c r="X5" s="19"/>
       <c r="Y5" s="42"/>
     </row>
-    <row r="6" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:48" ht="12.75" customHeight="1">
       <c r="B6" s="2" t="s">
         <v>282</v>
       </c>
       <c r="X6" s="19"/>
       <c r="Y6" s="42"/>
     </row>
-    <row r="7" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:48" ht="12.75" customHeight="1">
       <c r="B7" s="7" t="s">
         <v>283</v>
       </c>
@@ -3560,8 +3653,20 @@
       <c r="AR7" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="8" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS7" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT7" s="45" t="s">
+        <v>464</v>
+      </c>
+      <c r="AU7">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AV7" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="8" spans="2:48" ht="12.75" customHeight="1">
       <c r="B8" s="7" t="s">
         <v>284</v>
       </c>
@@ -3613,8 +3718,20 @@
       <c r="AR8" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="9" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS8" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT8" s="45" t="s">
+        <v>467</v>
+      </c>
+      <c r="AU8">
+        <v>12.9</v>
+      </c>
+      <c r="AV8" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="9" spans="2:48" ht="12.75" customHeight="1">
       <c r="B9" s="8" t="s">
         <v>349</v>
       </c>
@@ -3684,8 +3801,20 @@
       <c r="AR9" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="10" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS9" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT9" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="AU9">
+        <v>23.6</v>
+      </c>
+      <c r="AV9" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="10" spans="2:48" ht="12.75" customHeight="1">
       <c r="B10" s="7" t="s">
         <v>285</v>
       </c>
@@ -3740,7 +3869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:48" ht="12.75" customHeight="1">
       <c r="B11" s="7" t="s">
         <v>286</v>
       </c>
@@ -3766,7 +3895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:48" ht="12.75" customHeight="1">
       <c r="B12" s="7" t="s">
         <v>287</v>
       </c>
@@ -3792,7 +3921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:48" ht="12.75" customHeight="1">
       <c r="B13" s="7" t="s">
         <v>288</v>
       </c>
@@ -3856,8 +3985,17 @@
       <c r="AR13" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="14" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS13" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT13" s="45" t="s">
+        <v>470</v>
+      </c>
+      <c r="AV13" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="14" spans="2:48" ht="12.75" customHeight="1">
       <c r="B14" s="7" t="s">
         <v>289</v>
       </c>
@@ -3912,7 +4050,7 @@
       <c r="X14" s="39"/>
       <c r="Y14" s="42"/>
     </row>
-    <row r="15" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:48" ht="12.75" customHeight="1">
       <c r="B15" s="7" t="s">
         <v>290</v>
       </c>
@@ -3958,7 +4096,7 @@
       <c r="X15" s="39"/>
       <c r="Y15" s="42"/>
     </row>
-    <row r="16" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:48" ht="12.75" customHeight="1">
       <c r="B16" s="7" t="s">
         <v>291</v>
       </c>
@@ -3983,7 +4121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:48" ht="12.75" customHeight="1">
       <c r="B17" s="7" t="s">
         <v>292</v>
       </c>
@@ -4062,8 +4200,20 @@
       <c r="AR17" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="18" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS17" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT17" s="45" t="s">
+        <v>464</v>
+      </c>
+      <c r="AU17" s="45">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AV17" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="18" spans="2:48" ht="12.75" customHeight="1">
       <c r="B18" s="7" t="s">
         <v>293</v>
       </c>
@@ -4133,8 +4283,20 @@
       <c r="AR18" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="19" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS18" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT18" s="45" t="s">
+        <v>472</v>
+      </c>
+      <c r="AU18" s="45">
+        <v>10.9</v>
+      </c>
+      <c r="AV18" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="19" spans="2:48" ht="12.75" customHeight="1">
       <c r="B19" s="7" t="s">
         <v>294</v>
       </c>
@@ -4150,7 +4312,7 @@
       <c r="X19" s="19"/>
       <c r="Y19" s="42"/>
     </row>
-    <row r="20" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:48" ht="12.75" customHeight="1">
       <c r="B20" s="7" t="s">
         <v>295</v>
       </c>
@@ -4166,7 +4328,7 @@
       <c r="X20" s="19"/>
       <c r="Y20" s="42"/>
     </row>
-    <row r="21" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:48" ht="12.75" customHeight="1">
       <c r="B21" s="7" t="s">
         <v>296</v>
       </c>
@@ -4182,7 +4344,7 @@
       <c r="X21" s="19"/>
       <c r="Y21" s="42"/>
     </row>
-    <row r="22" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:48" ht="12.75" customHeight="1">
       <c r="B22" s="7" t="s">
         <v>297</v>
       </c>
@@ -4198,7 +4360,7 @@
       <c r="X22" s="19"/>
       <c r="Y22" s="42"/>
     </row>
-    <row r="23" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:48" ht="12.75" customHeight="1">
       <c r="B23" s="7" t="s">
         <v>298</v>
       </c>
@@ -4223,7 +4385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:48" ht="12.75" customHeight="1">
       <c r="B24" s="7" t="s">
         <v>299</v>
       </c>
@@ -4278,7 +4440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:48" ht="12.75" customHeight="1">
       <c r="B25" s="7" t="s">
         <v>300</v>
       </c>
@@ -4303,7 +4465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:48" ht="12.75" customHeight="1">
       <c r="B26" s="7" t="s">
         <v>301</v>
       </c>
@@ -4313,8 +4475,8 @@
       <c r="X26" s="20"/>
       <c r="Y26" s="42"/>
     </row>
-    <row r="27" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="51" t="s">
+    <row r="27" spans="2:48" ht="12.75" customHeight="1">
+      <c r="B27" s="49" t="s">
         <v>310</v>
       </c>
       <c r="I27" s="7" t="s">
@@ -4350,11 +4512,11 @@
       <c r="X27" s="20"/>
       <c r="Y27" s="42"/>
     </row>
-    <row r="28" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:48" ht="12.75" customHeight="1">
       <c r="X28" s="19"/>
       <c r="Y28" s="42"/>
     </row>
-    <row r="29" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:48" ht="12.75" customHeight="1">
       <c r="B29" s="7" t="s">
         <v>302</v>
       </c>
@@ -4418,7 +4580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:48" ht="12.75" customHeight="1">
       <c r="B30" s="21" t="s">
         <v>431</v>
       </c>
@@ -4506,8 +4668,20 @@
       <c r="AR30" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="31" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS30" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT30" s="45" t="s">
+        <v>473</v>
+      </c>
+      <c r="AU30" s="45">
+        <v>23.7</v>
+      </c>
+      <c r="AV30" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="31" spans="2:48" ht="12.75" customHeight="1">
       <c r="B31" s="21" t="s">
         <v>432</v>
       </c>
@@ -4589,8 +4763,20 @@
       <c r="AR31" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="32" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS31" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT31" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="AU31" s="54">
+        <v>20</v>
+      </c>
+      <c r="AV31" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="32" spans="2:48" ht="12.75" customHeight="1">
       <c r="B32" s="7" t="s">
         <v>303</v>
       </c>
@@ -4630,7 +4816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:48" ht="12.75" customHeight="1">
       <c r="B33" s="7" t="s">
         <v>304</v>
       </c>
@@ -4688,11 +4874,23 @@
       <c r="AQ33" s="22" t="s">
         <v>436</v>
       </c>
-      <c r="AR33" t="s">
+      <c r="AR33" s="45" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="34" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS33" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT33" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="AU33" s="54">
+        <v>20</v>
+      </c>
+      <c r="AV33" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="34" spans="2:48" ht="12.75" customHeight="1">
       <c r="B34" s="7" t="s">
         <v>305</v>
       </c>
@@ -4744,8 +4942,20 @@
       <c r="AR34" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="35" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS34" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT34" s="45" t="s">
+        <v>475</v>
+      </c>
+      <c r="AU34" s="54">
+        <v>12</v>
+      </c>
+      <c r="AV34" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="35" spans="2:48" ht="12.75" customHeight="1">
       <c r="B35" s="21" t="s">
         <v>437</v>
       </c>
@@ -4786,7 +4996,7 @@
       </c>
       <c r="AQ35" s="22"/>
     </row>
-    <row r="36" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:48" ht="12.75" customHeight="1">
       <c r="B36" s="21" t="s">
         <v>438</v>
       </c>
@@ -4818,7 +5028,7 @@
       </c>
       <c r="AQ36" s="22"/>
     </row>
-    <row r="37" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:48" ht="12.75" customHeight="1">
       <c r="B37" s="21" t="s">
         <v>439</v>
       </c>
@@ -4838,7 +5048,7 @@
       <c r="Y37" s="42"/>
       <c r="AQ37" s="22"/>
     </row>
-    <row r="38" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:48" ht="12.75" customHeight="1">
       <c r="B38" s="7" t="s">
         <v>306</v>
       </c>
@@ -4866,18 +5076,18 @@
       <c r="X38" s="20"/>
       <c r="Y38" s="42"/>
     </row>
-    <row r="39" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:48" ht="12.75" customHeight="1">
       <c r="X39" s="19"/>
       <c r="Y39" s="42"/>
     </row>
-    <row r="40" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:48" ht="12.75" customHeight="1">
       <c r="B40" s="2" t="s">
         <v>307</v>
       </c>
       <c r="X40" s="19"/>
       <c r="Y40" s="42"/>
     </row>
-    <row r="41" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:48" ht="12.75" customHeight="1">
       <c r="B41" s="7" t="s">
         <v>291</v>
       </c>
@@ -4893,7 +5103,7 @@
       <c r="X41" s="19"/>
       <c r="Y41" s="42"/>
     </row>
-    <row r="42" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:48" ht="12.75" customHeight="1">
       <c r="B42" s="7" t="s">
         <v>298</v>
       </c>
@@ -4948,7 +5158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:48" ht="12.75" customHeight="1">
       <c r="B43" s="7" t="s">
         <v>308</v>
       </c>
@@ -4964,7 +5174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:48" ht="12.75" customHeight="1">
       <c r="B44" s="7" t="s">
         <v>299</v>
       </c>
@@ -4998,7 +5208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:48" ht="12.75" customHeight="1">
       <c r="B45" s="7" t="s">
         <v>300</v>
       </c>
@@ -5023,7 +5233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:48" ht="12.75" customHeight="1">
       <c r="B46" s="7" t="s">
         <v>309</v>
       </c>
@@ -5039,7 +5249,7 @@
       <c r="X46" s="19"/>
       <c r="Y46" s="42"/>
     </row>
-    <row r="47" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:48" ht="12.75" customHeight="1">
       <c r="B47" s="7" t="s">
         <v>310</v>
       </c>
@@ -5082,7 +5292,7 @@
       <c r="X47" s="31" t="s">
         <v>361</v>
       </c>
-      <c r="Y47" s="50" t="s">
+      <c r="Y47" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA47" s="7" t="s">
@@ -5109,8 +5319,18 @@
       <c r="AR47" s="22" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="48" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS47" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT47" s="45" t="s">
+        <v>470</v>
+      </c>
+      <c r="AU47" s="45"/>
+      <c r="AV47" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="48" spans="2:48" ht="12.75" customHeight="1">
       <c r="B48" s="7" t="s">
         <v>294</v>
       </c>
@@ -5126,7 +5346,7 @@
       <c r="X48" s="19"/>
       <c r="Y48" s="42"/>
     </row>
-    <row r="49" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:48" ht="12.75" customHeight="1">
       <c r="B49" s="7" t="s">
         <v>295</v>
       </c>
@@ -5142,7 +5362,7 @@
       <c r="X49" s="19"/>
       <c r="Y49" s="42"/>
     </row>
-    <row r="50" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:48" ht="12.75" customHeight="1">
       <c r="B50" s="7" t="s">
         <v>296</v>
       </c>
@@ -5158,7 +5378,7 @@
       <c r="X50" s="19"/>
       <c r="Y50" s="42"/>
     </row>
-    <row r="51" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:48" ht="12.75" customHeight="1">
       <c r="B51" s="7" t="s">
         <v>297</v>
       </c>
@@ -5174,18 +5394,18 @@
       <c r="X51" s="19"/>
       <c r="Y51" s="42"/>
     </row>
-    <row r="52" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:48" ht="12.75" customHeight="1">
       <c r="X52" s="19"/>
       <c r="Y52" s="42"/>
     </row>
-    <row r="53" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:48" ht="12.75" customHeight="1">
       <c r="B53" s="2" t="s">
         <v>311</v>
       </c>
       <c r="X53" s="19"/>
       <c r="Y53" s="42"/>
     </row>
-    <row r="54" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:48" ht="12.75" customHeight="1">
       <c r="B54" s="7" t="s">
         <v>312</v>
       </c>
@@ -5213,7 +5433,7 @@
       <c r="X54" s="20"/>
       <c r="Y54" s="42"/>
     </row>
-    <row r="55" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:48" ht="12.75" customHeight="1">
       <c r="B55" s="7" t="s">
         <v>313</v>
       </c>
@@ -5247,7 +5467,7 @@
       <c r="X55" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="Y55" s="50" t="s">
+      <c r="Y55" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA55" s="7" t="s">
@@ -5262,8 +5482,18 @@
       <c r="AR55" s="22" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="56" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS55" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT55" s="45" t="s">
+        <v>476</v>
+      </c>
+      <c r="AU55" s="45"/>
+      <c r="AV55" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="56" spans="2:48" ht="12.75" customHeight="1">
       <c r="B56" s="7" t="s">
         <v>314</v>
       </c>
@@ -5291,7 +5521,7 @@
       <c r="X56" s="20"/>
       <c r="Y56" s="42"/>
     </row>
-    <row r="57" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:48" ht="12.75" customHeight="1">
       <c r="B57" s="21" t="s">
         <v>388</v>
       </c>
@@ -5334,8 +5564,14 @@
       <c r="AR57" s="22" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="58" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS57" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT57" s="45" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="58" spans="2:48" ht="12.75" customHeight="1">
       <c r="B58" s="21" t="s">
         <v>389</v>
       </c>
@@ -5378,8 +5614,14 @@
       <c r="AR58" s="22" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="59" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS58" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT58" s="45" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="59" spans="2:48" ht="12.75" customHeight="1">
       <c r="B59" s="7" t="s">
         <v>315</v>
       </c>
@@ -5415,7 +5657,7 @@
       </c>
       <c r="Y59" s="42"/>
     </row>
-    <row r="60" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:48" ht="12.75" customHeight="1">
       <c r="B60" s="6" t="s">
         <v>316</v>
       </c>
@@ -5446,7 +5688,7 @@
       <c r="X60" s="31" t="s">
         <v>364</v>
       </c>
-      <c r="Y60" s="50" t="s">
+      <c r="Y60" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA60" s="7" t="s">
@@ -5473,8 +5715,14 @@
       <c r="AR60" s="22" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="61" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS60" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT60" s="45" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="61" spans="2:48" ht="12.75" customHeight="1">
       <c r="B61" s="6" t="s">
         <v>317</v>
       </c>
@@ -5517,7 +5765,7 @@
       <c r="X61" s="31" t="s">
         <v>365</v>
       </c>
-      <c r="Y61" s="50" t="s">
+      <c r="Y61" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA61" s="7" t="s">
@@ -5550,8 +5798,20 @@
       <c r="AR61" s="22" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="62" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS61" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT61" s="45" t="s">
+        <v>478</v>
+      </c>
+      <c r="AU61" s="45" t="s">
+        <v>479</v>
+      </c>
+      <c r="AV61" s="45" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="62" spans="2:48" ht="12.75" customHeight="1">
       <c r="B62" s="6" t="s">
         <v>318</v>
       </c>
@@ -5585,18 +5845,30 @@
       <c r="X62" s="31" t="s">
         <v>366</v>
       </c>
-      <c r="Y62" s="50" t="s">
+      <c r="Y62" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AR62" s="22" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="63" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS62" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT62" s="45" t="s">
+        <v>481</v>
+      </c>
+      <c r="AU62">
+        <v>947.249146</v>
+      </c>
+      <c r="AV62" s="45" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="63" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="X63" s="19"/>
       <c r="Y63" s="42"/>
     </row>
-    <row r="64" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B64" s="24" t="s">
         <v>98</v>
       </c>
@@ -5604,7 +5876,7 @@
       <c r="X64" s="19"/>
       <c r="Y64" s="42"/>
     </row>
-    <row r="65" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B65" s="26" t="s">
         <v>371</v>
       </c>
@@ -5648,7 +5920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B66" s="28" t="s">
         <v>374</v>
       </c>
@@ -5674,7 +5946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B67" s="7" t="s">
         <v>102</v>
       </c>
@@ -5699,7 +5971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B68" s="7" t="s">
         <v>373</v>
       </c>
@@ -5724,7 +5996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B69" s="7" t="s">
         <v>372</v>
       </c>
@@ -5758,7 +6030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B70" s="7" t="s">
         <v>107</v>
       </c>
@@ -5780,7 +6052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B71" s="6" t="s">
         <v>375</v>
       </c>
@@ -5814,7 +6086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B72" s="7" t="s">
         <v>376</v>
       </c>
@@ -5837,18 +6109,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:48" ht="12.75" customHeight="1">
       <c r="X73" s="19"/>
       <c r="Y73" s="42"/>
     </row>
-    <row r="74" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:48" ht="12.75" customHeight="1">
       <c r="B74" s="2" t="s">
         <v>319</v>
       </c>
       <c r="X74" s="19"/>
       <c r="Y74" s="42"/>
     </row>
-    <row r="75" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:48" ht="12.75" customHeight="1">
       <c r="B75" s="8" t="s">
         <v>350</v>
       </c>
@@ -5891,7 +6163,7 @@
       <c r="X75" s="31" t="s">
         <v>455</v>
       </c>
-      <c r="Y75" s="50" t="s">
+      <c r="Y75" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA75" s="7" t="s">
@@ -5909,8 +6181,17 @@
       <c r="AR75" s="22" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="76" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS75" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT75" s="45" t="s">
+        <v>482</v>
+      </c>
+      <c r="AU75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:48" ht="12.75" customHeight="1">
       <c r="B76" s="21" t="s">
         <v>435</v>
       </c>
@@ -5953,7 +6234,7 @@
       <c r="X76" s="31" t="s">
         <v>367</v>
       </c>
-      <c r="Y76" s="50" t="s">
+      <c r="Y76" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA76" s="7" t="s">
@@ -5971,8 +6252,17 @@
       <c r="AR76" s="22" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="77" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS76" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT76" s="45" t="s">
+        <v>482</v>
+      </c>
+      <c r="AU76" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:48" ht="12.75" customHeight="1">
       <c r="B77" s="7" t="s">
         <v>320</v>
       </c>
@@ -6006,7 +6296,7 @@
       <c r="X77" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="Y77" s="50" t="s">
+      <c r="Y77" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA77" s="7" t="s">
@@ -6024,8 +6314,18 @@
       <c r="AR77" s="22" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="78" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS77" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT77" s="45" t="s">
+        <v>476</v>
+      </c>
+      <c r="AU77" s="45"/>
+      <c r="AV77" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="78" spans="2:48" ht="12.75" customHeight="1">
       <c r="B78" s="7" t="s">
         <v>321</v>
       </c>
@@ -6041,7 +6341,7 @@
       <c r="X78" s="19"/>
       <c r="Y78" s="42"/>
     </row>
-    <row r="79" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:48" ht="12.75" customHeight="1">
       <c r="B79" s="7" t="s">
         <v>322</v>
       </c>
@@ -6057,7 +6357,7 @@
       <c r="X79" s="19"/>
       <c r="Y79" s="42"/>
     </row>
-    <row r="80" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:48" ht="12.75" customHeight="1">
       <c r="B80" s="7" t="s">
         <v>323</v>
       </c>
@@ -6094,7 +6394,7 @@
       <c r="X80" s="39"/>
       <c r="Y80" s="42"/>
     </row>
-    <row r="81" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:48" ht="12.75" customHeight="1">
       <c r="B81" s="7" t="s">
         <v>324</v>
       </c>
@@ -6128,7 +6428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:48" ht="12.75" customHeight="1">
       <c r="B82" s="7" t="s">
         <v>325</v>
       </c>
@@ -6144,7 +6444,7 @@
       <c r="X82" s="19"/>
       <c r="Y82" s="42"/>
     </row>
-    <row r="83" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:48" ht="12.75" customHeight="1">
       <c r="B83" s="7" t="s">
         <v>326</v>
       </c>
@@ -6178,7 +6478,7 @@
       <c r="X83" s="20" t="s">
         <v>369</v>
       </c>
-      <c r="Y83" s="50" t="s">
+      <c r="Y83" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA83" s="7" t="s">
@@ -6196,8 +6496,18 @@
       <c r="AR83" s="22" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="84" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS83" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT83" s="45" t="s">
+        <v>476</v>
+      </c>
+      <c r="AU83" s="45"/>
+      <c r="AV83" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="84" spans="2:48" ht="12.75" customHeight="1">
       <c r="B84" s="7" t="s">
         <v>327</v>
       </c>
@@ -6213,7 +6523,7 @@
       <c r="X84" s="19"/>
       <c r="Y84" s="42"/>
     </row>
-    <row r="85" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:48" ht="12.75" customHeight="1">
       <c r="B85" s="7" t="s">
         <v>328</v>
       </c>
@@ -6229,7 +6539,7 @@
       <c r="X85" s="19"/>
       <c r="Y85" s="42"/>
     </row>
-    <row r="86" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:48" ht="12.75" customHeight="1">
       <c r="B86" s="7" t="s">
         <v>329</v>
       </c>
@@ -6254,7 +6564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:48" ht="12.75" customHeight="1">
       <c r="B87" s="7" t="s">
         <v>330</v>
       </c>
@@ -6279,18 +6589,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:48" ht="12.75" customHeight="1">
       <c r="X88" s="19"/>
       <c r="Y88" s="42"/>
     </row>
-    <row r="89" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:48" ht="12.75" customHeight="1">
       <c r="B89" s="2" t="s">
         <v>331</v>
       </c>
       <c r="X89" s="19"/>
       <c r="Y89" s="42"/>
     </row>
-    <row r="90" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:48" ht="12.75" customHeight="1">
       <c r="B90" s="7" t="s">
         <v>332</v>
       </c>
@@ -6345,7 +6655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:48" ht="12.75" customHeight="1">
       <c r="B91" s="7" t="s">
         <v>333</v>
       </c>
@@ -6397,7 +6707,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:48" ht="12.75" customHeight="1">
       <c r="B92" s="7" t="s">
         <v>334</v>
       </c>
@@ -6421,7 +6731,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:48" ht="12.75" customHeight="1">
       <c r="B93" s="7" t="s">
         <v>335</v>
       </c>
@@ -6435,7 +6745,7 @@
       <c r="X93" s="19"/>
       <c r="Y93" s="42"/>
     </row>
-    <row r="94" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:48" ht="12.75" customHeight="1">
       <c r="B94" s="7" t="s">
         <v>336</v>
       </c>
@@ -6490,7 +6800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:48" ht="12.75" customHeight="1">
       <c r="B95" s="7" t="s">
         <v>337</v>
       </c>
@@ -6527,18 +6837,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="X96" s="19"/>
       <c r="Y96" s="42"/>
     </row>
-    <row r="97" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B97" s="2" t="s">
         <v>338</v>
       </c>
       <c r="X97" s="19"/>
       <c r="Y97" s="42"/>
     </row>
-    <row r="98" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B98" s="6" t="s">
         <v>339</v>
       </c>
@@ -6581,22 +6891,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="X99" s="19"/>
       <c r="Y99" s="42"/>
     </row>
-    <row r="100" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:48" ht="12.75" customHeight="1">
       <c r="X100" s="19"/>
       <c r="Y100" s="42"/>
     </row>
-    <row r="101" spans="2:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:48" ht="24.75" customHeight="1">
       <c r="B101" s="34" t="s">
         <v>398</v>
       </c>
       <c r="X101" s="19"/>
       <c r="Y101" s="42"/>
     </row>
-    <row r="102" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:48" ht="12.75" customHeight="1">
       <c r="B102" s="7" t="s">
         <v>340</v>
       </c>
@@ -6635,7 +6945,7 @@
       <c r="X102" s="31" t="s">
         <v>393</v>
       </c>
-      <c r="Y102" s="50" t="s">
+      <c r="Y102" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA102" s="7" t="s">
@@ -6659,7 +6969,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="103" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:48" ht="12.75" customHeight="1">
       <c r="B103" s="21" t="s">
         <v>379</v>
       </c>
@@ -6702,7 +7012,7 @@
       <c r="X103" s="31" t="s">
         <v>396</v>
       </c>
-      <c r="Y103" s="50" t="s">
+      <c r="Y103" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA103" s="7" t="s">
@@ -6721,7 +7031,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="104" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:48" ht="12.75" customHeight="1">
       <c r="B104" s="21" t="s">
         <v>380</v>
       </c>
@@ -6764,7 +7074,7 @@
       <c r="X104" s="31" t="s">
         <v>397</v>
       </c>
-      <c r="Y104" s="50" t="s">
+      <c r="Y104" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA104" s="7" t="s">
@@ -6783,7 +7093,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="105" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:48" ht="12.75" customHeight="1">
       <c r="B105" t="s">
         <v>341</v>
       </c>
@@ -6817,7 +7127,7 @@
       <c r="X105" s="35" t="s">
         <v>399</v>
       </c>
-      <c r="Y105" s="50" t="s">
+      <c r="Y105" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AQ105" s="29" t="s">
@@ -6827,7 +7137,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="106" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:48" ht="12.75" customHeight="1">
       <c r="B106" t="s">
         <v>342</v>
       </c>
@@ -6867,7 +7177,7 @@
       <c r="X106" s="31" t="s">
         <v>400</v>
       </c>
-      <c r="Y106" s="50" t="s">
+      <c r="Y106" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AQ106" s="22" t="s">
@@ -6877,7 +7187,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="107" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:48" ht="12.75" customHeight="1">
       <c r="B107" t="s">
         <v>343</v>
       </c>
@@ -6911,7 +7221,7 @@
       <c r="X107" s="31" t="s">
         <v>404</v>
       </c>
-      <c r="Y107" s="50" t="s">
+      <c r="Y107" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AQ107" s="7" t="s">
@@ -6921,7 +7231,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="108" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:48" ht="12.75" customHeight="1">
       <c r="B108" s="22" t="s">
         <v>386</v>
       </c>
@@ -6955,7 +7265,7 @@
       <c r="X108" s="31" t="s">
         <v>405</v>
       </c>
-      <c r="Y108" s="50" t="s">
+      <c r="Y108" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AQ108" s="7" t="s">
@@ -6965,7 +7275,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="109" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:48" ht="12.75" customHeight="1">
       <c r="B109" t="s">
         <v>345</v>
       </c>
@@ -6990,7 +7300,7 @@
       <c r="X109" s="31" t="s">
         <v>459</v>
       </c>
-      <c r="Y109" s="50" t="s">
+      <c r="Y109" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AM109" s="7"/>
@@ -7003,7 +7313,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="110" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:48" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B110" s="22" t="s">
         <v>444</v>
       </c>
@@ -7022,7 +7332,7 @@
       <c r="X110" s="31" t="s">
         <v>407</v>
       </c>
-      <c r="Y110" s="50" t="s">
+      <c r="Y110" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AM110" s="7"/>
@@ -7034,15 +7344,27 @@
       <c r="AR110" s="22" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="111" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS110" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT110" s="45" t="s">
+        <v>484</v>
+      </c>
+      <c r="AU110" s="16">
+        <v>-20.6</v>
+      </c>
+      <c r="AV110" s="45" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="111" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B111" s="5" t="s">
         <v>346</v>
       </c>
       <c r="X111" s="19"/>
       <c r="Y111" s="42"/>
     </row>
-    <row r="112" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B112" t="s">
         <v>343</v>
       </c>
@@ -7058,7 +7380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B113" t="s">
         <v>344</v>
       </c>
@@ -7074,7 +7396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B114" t="s">
         <v>347</v>
       </c>
@@ -7090,7 +7412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B115" t="s">
         <v>341</v>
       </c>
@@ -7106,7 +7428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:48" ht="12.75" hidden="1" customHeight="1">
       <c r="B116" t="s">
         <v>342</v>
       </c>
@@ -7122,18 +7444,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:48" ht="12.75" customHeight="1">
       <c r="X117" s="19"/>
       <c r="Y117" s="42"/>
     </row>
-    <row r="118" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:48" ht="12.75" customHeight="1">
       <c r="B118" s="38" t="s">
         <v>412</v>
       </c>
       <c r="X118" s="19"/>
       <c r="Y118" s="42"/>
     </row>
-    <row r="119" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:48" ht="12.75" customHeight="1">
       <c r="B119" s="21" t="s">
         <v>409</v>
       </c>
@@ -7177,7 +7499,7 @@
       <c r="X119" s="31" t="s">
         <v>419</v>
       </c>
-      <c r="Y119" s="50" t="s">
+      <c r="Y119" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA119" s="7" t="s">
@@ -7193,8 +7515,17 @@
       <c r="AR119" s="22" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="120" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS119" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT119" s="45" t="s">
+        <v>483</v>
+      </c>
+      <c r="AU119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="2:48" ht="12.75" customHeight="1">
       <c r="B120" s="21" t="s">
         <v>410</v>
       </c>
@@ -7228,7 +7559,7 @@
       <c r="X120" s="31" t="s">
         <v>420</v>
       </c>
-      <c r="Y120" s="50" t="s">
+      <c r="Y120" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA120" s="7" t="s">
@@ -7246,8 +7577,20 @@
       <c r="AR120" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="121" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS120" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT120" s="45" t="s">
+        <v>467</v>
+      </c>
+      <c r="AU120" s="45">
+        <v>12.9</v>
+      </c>
+      <c r="AV120" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="121" spans="2:48" ht="12.75" customHeight="1">
       <c r="B121" s="21" t="s">
         <v>348</v>
       </c>
@@ -7284,7 +7627,7 @@
       <c r="X121" s="31" t="s">
         <v>421</v>
       </c>
-      <c r="Y121" s="50" t="s">
+      <c r="Y121" s="48" t="s">
         <v>352</v>
       </c>
       <c r="AA121" s="7" t="s">
@@ -7294,9 +7637,24 @@
       <c r="AC121" s="7">
         <v>1</v>
       </c>
-      <c r="AQ121" s="22"/>
-    </row>
-    <row r="122" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AQ121" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR121" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="AS121" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT121" s="45" t="s">
+        <v>482</v>
+      </c>
+      <c r="AU121" s="45">
+        <v>0</v>
+      </c>
+      <c r="AV121" s="45"/>
+    </row>
+    <row r="122" spans="2:48" ht="12.75" customHeight="1">
       <c r="B122" s="21" t="s">
         <v>411</v>
       </c>
@@ -7326,7 +7684,9 @@
       <c r="X122" s="31" t="s">
         <v>422</v>
       </c>
-      <c r="Y122" s="42"/>
+      <c r="Y122" s="46" t="s">
+        <v>352</v>
+      </c>
       <c r="AA122" s="7" t="s">
         <v>157</v>
       </c>
@@ -7340,15 +7700,27 @@
       <c r="AR122" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="123" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS122" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT122" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="AU122" s="54">
+        <v>20</v>
+      </c>
+      <c r="AV122" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="123" spans="2:48" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B123" s="38" t="s">
         <v>413</v>
       </c>
       <c r="X123" s="19"/>
       <c r="Y123" s="42"/>
     </row>
-    <row r="124" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:48" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B124" s="21" t="s">
         <v>409</v>
       </c>
@@ -7392,7 +7764,10 @@
       <c r="X124" s="31" t="s">
         <v>423</v>
       </c>
-      <c r="Y124" s="42"/>
+      <c r="Y124" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z124" s="45"/>
       <c r="AA124" s="7" t="s">
         <v>154</v>
       </c>
@@ -7400,8 +7775,27 @@
       <c r="AC124" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD124" s="45"/>
+      <c r="AE124" s="45"/>
+      <c r="AF124" s="45"/>
+      <c r="AG124" s="45"/>
+      <c r="AH124" s="45"/>
+      <c r="AI124" s="45"/>
+      <c r="AJ124" s="45"/>
+      <c r="AK124" s="45"/>
+      <c r="AL124" s="45"/>
+      <c r="AM124" s="45"/>
+      <c r="AN124" s="45"/>
+      <c r="AO124" s="45"/>
+      <c r="AP124" s="45"/>
+      <c r="AQ124" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR124" s="22" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="125" spans="2:48" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B125" s="21" t="s">
         <v>410</v>
       </c>
@@ -7435,7 +7829,10 @@
       <c r="X125" s="31" t="s">
         <v>424</v>
       </c>
-      <c r="Y125" s="42"/>
+      <c r="Y125" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z125" s="45"/>
       <c r="AA125" s="7" t="s">
         <v>155</v>
       </c>
@@ -7445,14 +7842,27 @@
       <c r="AC125" s="7">
         <v>4</v>
       </c>
+      <c r="AD125" s="45"/>
+      <c r="AE125" s="45"/>
+      <c r="AF125" s="45"/>
+      <c r="AG125" s="45"/>
+      <c r="AH125" s="45"/>
+      <c r="AI125" s="45"/>
+      <c r="AJ125" s="45"/>
+      <c r="AK125" s="45"/>
+      <c r="AL125" s="45"/>
+      <c r="AM125" s="45"/>
+      <c r="AN125" s="45"/>
+      <c r="AO125" s="45"/>
+      <c r="AP125" s="45"/>
       <c r="AQ125" s="22" t="s">
         <v>415</v>
       </c>
-      <c r="AR125" s="16" t="s">
+      <c r="AR125" s="45" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="126" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:48" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B126" s="21" t="s">
         <v>348</v>
       </c>
@@ -7489,7 +7899,10 @@
       <c r="X126" s="31" t="s">
         <v>425</v>
       </c>
-      <c r="Y126" s="42"/>
+      <c r="Y126" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z126" s="45"/>
       <c r="AA126" s="7" t="s">
         <v>156</v>
       </c>
@@ -7497,9 +7910,27 @@
       <c r="AC126" s="7">
         <v>1</v>
       </c>
-      <c r="AQ126" s="22"/>
-    </row>
-    <row r="127" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD126" s="45"/>
+      <c r="AE126" s="45"/>
+      <c r="AF126" s="45"/>
+      <c r="AG126" s="45"/>
+      <c r="AH126" s="45"/>
+      <c r="AI126" s="45"/>
+      <c r="AJ126" s="45"/>
+      <c r="AK126" s="45"/>
+      <c r="AL126" s="45"/>
+      <c r="AM126" s="45"/>
+      <c r="AN126" s="45"/>
+      <c r="AO126" s="45"/>
+      <c r="AP126" s="45"/>
+      <c r="AQ126" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR126" s="45" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="127" spans="2:48" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B127" s="21" t="s">
         <v>411</v>
       </c>
@@ -7529,7 +7960,10 @@
       <c r="X127" s="31" t="s">
         <v>426</v>
       </c>
-      <c r="Y127" s="42"/>
+      <c r="Y127" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z127" s="45"/>
       <c r="AA127" s="7" t="s">
         <v>157</v>
       </c>
@@ -7537,21 +7971,34 @@
       <c r="AC127" s="7">
         <v>1</v>
       </c>
+      <c r="AD127" s="45"/>
+      <c r="AE127" s="45"/>
+      <c r="AF127" s="45"/>
+      <c r="AG127" s="45"/>
+      <c r="AH127" s="45"/>
+      <c r="AI127" s="45"/>
+      <c r="AJ127" s="45"/>
+      <c r="AK127" s="45"/>
+      <c r="AL127" s="45"/>
+      <c r="AM127" s="45"/>
+      <c r="AN127" s="45"/>
+      <c r="AO127" s="45"/>
+      <c r="AP127" s="45"/>
       <c r="AQ127" s="22" t="s">
         <v>418</v>
       </c>
-      <c r="AR127" s="16" t="s">
+      <c r="AR127" s="45" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="128" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:48" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B128" s="38" t="s">
         <v>414</v>
       </c>
       <c r="X128" s="19"/>
       <c r="Y128" s="42"/>
     </row>
-    <row r="129" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:46" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B129" s="21" t="s">
         <v>409</v>
       </c>
@@ -7595,7 +8042,10 @@
       <c r="X129" s="31" t="s">
         <v>427</v>
       </c>
-      <c r="Y129" s="42"/>
+      <c r="Y129" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z129" s="45"/>
       <c r="AA129" s="7" t="s">
         <v>154</v>
       </c>
@@ -7603,8 +8053,27 @@
       <c r="AC129" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD129" s="45"/>
+      <c r="AE129" s="45"/>
+      <c r="AF129" s="45"/>
+      <c r="AG129" s="45"/>
+      <c r="AH129" s="45"/>
+      <c r="AI129" s="45"/>
+      <c r="AJ129" s="45"/>
+      <c r="AK129" s="45"/>
+      <c r="AL129" s="45"/>
+      <c r="AM129" s="45"/>
+      <c r="AN129" s="45"/>
+      <c r="AO129" s="45"/>
+      <c r="AP129" s="45"/>
+      <c r="AQ129" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR129" s="22" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="130" spans="2:46" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B130" s="21" t="s">
         <v>410</v>
       </c>
@@ -7638,7 +8107,10 @@
       <c r="X130" s="31" t="s">
         <v>428</v>
       </c>
-      <c r="Y130" s="42"/>
+      <c r="Y130" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z130" s="45"/>
       <c r="AA130" s="7" t="s">
         <v>155</v>
       </c>
@@ -7648,14 +8120,27 @@
       <c r="AC130" s="7">
         <v>4</v>
       </c>
+      <c r="AD130" s="45"/>
+      <c r="AE130" s="45"/>
+      <c r="AF130" s="45"/>
+      <c r="AG130" s="45"/>
+      <c r="AH130" s="45"/>
+      <c r="AI130" s="45"/>
+      <c r="AJ130" s="45"/>
+      <c r="AK130" s="45"/>
+      <c r="AL130" s="45"/>
+      <c r="AM130" s="45"/>
+      <c r="AN130" s="45"/>
+      <c r="AO130" s="45"/>
+      <c r="AP130" s="45"/>
       <c r="AQ130" s="22" t="s">
         <v>415</v>
       </c>
-      <c r="AR130" s="16" t="s">
+      <c r="AR130" s="45" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="131" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:46" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B131" s="21" t="s">
         <v>348</v>
       </c>
@@ -7692,7 +8177,10 @@
       <c r="X131" s="31" t="s">
         <v>429</v>
       </c>
-      <c r="Y131" s="42"/>
+      <c r="Y131" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z131" s="45"/>
       <c r="AA131" s="7" t="s">
         <v>156</v>
       </c>
@@ -7700,9 +8188,27 @@
       <c r="AC131" s="7">
         <v>1</v>
       </c>
-      <c r="AQ131" s="22"/>
-    </row>
-    <row r="132" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD131" s="45"/>
+      <c r="AE131" s="45"/>
+      <c r="AF131" s="45"/>
+      <c r="AG131" s="45"/>
+      <c r="AH131" s="45"/>
+      <c r="AI131" s="45"/>
+      <c r="AJ131" s="45"/>
+      <c r="AK131" s="45"/>
+      <c r="AL131" s="45"/>
+      <c r="AM131" s="45"/>
+      <c r="AN131" s="45"/>
+      <c r="AO131" s="45"/>
+      <c r="AP131" s="45"/>
+      <c r="AQ131" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR131" s="45" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="132" spans="2:46" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B132" s="21" t="s">
         <v>411</v>
       </c>
@@ -7732,7 +8238,10 @@
       <c r="X132" s="31" t="s">
         <v>430</v>
       </c>
-      <c r="Y132" s="42"/>
+      <c r="Y132" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z132" s="45"/>
       <c r="AA132" s="7" t="s">
         <v>157</v>
       </c>
@@ -7740,14 +8249,27 @@
       <c r="AC132" s="7">
         <v>1</v>
       </c>
+      <c r="AD132" s="45"/>
+      <c r="AE132" s="45"/>
+      <c r="AF132" s="45"/>
+      <c r="AG132" s="45"/>
+      <c r="AH132" s="45"/>
+      <c r="AI132" s="45"/>
+      <c r="AJ132" s="45"/>
+      <c r="AK132" s="45"/>
+      <c r="AL132" s="45"/>
+      <c r="AM132" s="45"/>
+      <c r="AN132" s="45"/>
+      <c r="AO132" s="45"/>
+      <c r="AP132" s="45"/>
       <c r="AQ132" s="22" t="s">
         <v>418</v>
       </c>
-      <c r="AR132" s="16" t="s">
+      <c r="AR132" s="45" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="133" spans="2:44" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:46" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B133" s="21"/>
       <c r="E133" s="7"/>
       <c r="F133" s="7"/>
@@ -7761,7 +8283,7 @@
       <c r="AC133" s="7"/>
       <c r="AQ133" s="22"/>
     </row>
-    <row r="134" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:46" ht="12.75" customHeight="1">
       <c r="B134" s="7"/>
       <c r="E134" s="7" t="s">
         <v>158</v>
@@ -7790,7 +8312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:46" ht="12.75" customHeight="1">
       <c r="B135" s="7"/>
       <c r="E135" s="7" t="s">
         <v>159</v>
@@ -7834,7 +8356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:46" ht="12.75" customHeight="1">
       <c r="B136" s="7"/>
       <c r="E136" s="7" t="s">
         <v>160</v>
@@ -7870,17 +8392,26 @@
       <c r="AC136" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AR136" s="45" t="s">
+        <v>451</v>
+      </c>
+      <c r="AS136" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT136" s="45" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="137" spans="2:46" ht="12.75" customHeight="1">
       <c r="Y137" s="42"/>
     </row>
-    <row r="138" spans="2:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:46" hidden="1">
       <c r="B138" s="2" t="s">
         <v>161</v>
       </c>
       <c r="Y138" s="42"/>
     </row>
-    <row r="139" spans="2:44" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:46" ht="25.5" hidden="1">
       <c r="B139" s="7" t="s">
         <v>162</v>
       </c>
@@ -7895,7 +8426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="2:44" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:46" ht="25.5" hidden="1">
       <c r="B140" s="7" t="s">
         <v>164</v>
       </c>
@@ -7910,7 +8441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="2:44" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:46" ht="25.5" hidden="1">
       <c r="B141" s="7" t="s">
         <v>166</v>
       </c>
@@ -7925,7 +8456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="2:44" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:46" ht="25.5" hidden="1">
       <c r="B142" s="7" t="s">
         <v>168</v>
       </c>
@@ -7940,7 +8471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="2:44" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:46" ht="25.5" hidden="1">
       <c r="B143" s="7" t="s">
         <v>170</v>
       </c>
@@ -7955,7 +8486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="2:44" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:46" ht="25.5" hidden="1">
       <c r="B144" s="7" t="s">
         <v>172</v>
       </c>
@@ -7970,7 +8501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:37" ht="25.5" hidden="1">
       <c r="B145" t="s">
         <v>174</v>
       </c>
@@ -7985,7 +8516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:37" ht="25.5" hidden="1">
       <c r="B146" s="7" t="s">
         <v>176</v>
       </c>
@@ -8000,7 +8531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:37" ht="25.5" hidden="1">
       <c r="B147" s="7" t="s">
         <v>178</v>
       </c>
@@ -8015,7 +8546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:37" ht="25.5" hidden="1">
       <c r="B148" s="7" t="s">
         <v>180</v>
       </c>
@@ -8030,7 +8561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:37" ht="25.5" hidden="1">
       <c r="B149" s="7" t="s">
         <v>182</v>
       </c>
@@ -8045,7 +8576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:37" ht="25.5" hidden="1">
       <c r="B150" s="7" t="s">
         <v>184</v>
       </c>
@@ -8060,7 +8591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:37" ht="25.5" hidden="1">
       <c r="B151" s="7" t="s">
         <v>186</v>
       </c>
@@ -8075,7 +8606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:37" ht="25.5" hidden="1">
       <c r="B152" s="7" t="s">
         <v>188</v>
       </c>
@@ -8090,7 +8621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:37" ht="25.5" hidden="1">
       <c r="B153" s="7" t="s">
         <v>190</v>
       </c>
@@ -8105,7 +8636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:37" ht="25.5" hidden="1">
       <c r="B154" s="7" t="s">
         <v>192</v>
       </c>
@@ -8120,7 +8651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:37" ht="25.5" hidden="1">
       <c r="B155" s="7" t="s">
         <v>194</v>
       </c>
@@ -8135,7 +8666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:37" ht="25.5" hidden="1">
       <c r="B156" s="7" t="s">
         <v>196</v>
       </c>
@@ -8150,7 +8681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:37" ht="25.5" hidden="1">
       <c r="B157" s="7" t="s">
         <v>198</v>
       </c>
@@ -8165,7 +8696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:37" ht="25.5" hidden="1">
       <c r="B158" s="7" t="s">
         <v>200</v>
       </c>
@@ -8177,7 +8708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:37" ht="25.5" hidden="1">
       <c r="B159" s="7" t="s">
         <v>202</v>
       </c>
@@ -8189,7 +8720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:37" ht="25.5" hidden="1">
       <c r="B160" s="7" t="s">
         <v>204</v>
       </c>
@@ -8201,7 +8732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:37" ht="25.5" hidden="1">
       <c r="B161" s="7" t="s">
         <v>206</v>
       </c>
@@ -8213,7 +8744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:37" ht="25.5" hidden="1">
       <c r="B162" s="7" t="s">
         <v>208</v>
       </c>
@@ -8225,7 +8756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:37" ht="25.5" hidden="1">
       <c r="B163" s="7" t="s">
         <v>210</v>
       </c>
@@ -8237,7 +8768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:37" ht="25.5" hidden="1">
       <c r="B164" s="7" t="s">
         <v>212</v>
       </c>
@@ -8249,7 +8780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:37" ht="25.5" hidden="1">
       <c r="B165" s="7" t="s">
         <v>214</v>
       </c>
@@ -8261,7 +8792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:37" ht="25.5" hidden="1">
       <c r="B166" s="7" t="s">
         <v>216</v>
       </c>
@@ -8273,7 +8804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:37" ht="25.5" hidden="1">
       <c r="B167" s="7" t="s">
         <v>218</v>
       </c>
@@ -8285,7 +8816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:37" ht="25.5" hidden="1">
       <c r="B168" s="7" t="s">
         <v>220</v>
       </c>
@@ -8297,7 +8828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:37" ht="25.5" hidden="1">
       <c r="B169" s="7" t="s">
         <v>222</v>
       </c>
@@ -8309,7 +8840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:37" ht="25.5" hidden="1">
       <c r="B170" s="7" t="s">
         <v>224</v>
       </c>
@@ -8324,7 +8855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:37" ht="25.5" hidden="1">
       <c r="B171" s="1" t="s">
         <v>226</v>
       </c>
@@ -8339,7 +8870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:37" ht="25.5" hidden="1">
       <c r="B172" s="1" t="s">
         <v>228</v>
       </c>
@@ -8354,7 +8885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:37" ht="25.5" hidden="1">
       <c r="B173" s="7" t="s">
         <v>230</v>
       </c>
@@ -8369,7 +8900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:37" ht="25.5" hidden="1">
       <c r="B174" s="7" t="s">
         <v>232</v>
       </c>
@@ -8384,7 +8915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:37" ht="25.5" hidden="1">
       <c r="B175" s="7" t="s">
         <v>234</v>
       </c>
@@ -8399,7 +8930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="2:37" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:37" ht="25.5" hidden="1">
       <c r="B176" s="7" t="s">
         <v>236</v>
       </c>
@@ -8414,7 +8945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:41" ht="25.5" hidden="1">
       <c r="B177" s="7" t="s">
         <v>238</v>
       </c>
@@ -8429,7 +8960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:41" ht="25.5" hidden="1">
       <c r="B178" s="7" t="s">
         <v>240</v>
       </c>
@@ -8444,7 +8975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:41" ht="25.5" hidden="1">
       <c r="B179" s="7" t="s">
         <v>242</v>
       </c>
@@ -8459,7 +8990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:41" ht="25.5" hidden="1">
       <c r="B180" s="7" t="s">
         <v>244</v>
       </c>
@@ -8474,7 +9005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:41" ht="25.5" hidden="1">
       <c r="B181" s="7" t="s">
         <v>246</v>
       </c>
@@ -8489,17 +9020,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="2:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:41" hidden="1">
       <c r="B182" s="7"/>
       <c r="Y182" s="42"/>
     </row>
-    <row r="183" spans="2:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:41" hidden="1">
       <c r="B183" s="2" t="s">
         <v>248</v>
       </c>
       <c r="Y183" s="42"/>
     </row>
-    <row r="184" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:41" ht="25.5" hidden="1">
       <c r="B184" s="7" t="s">
         <v>249</v>
       </c>
@@ -8514,7 +9045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:41" ht="25.5" hidden="1">
       <c r="B185" s="7" t="s">
         <v>250</v>
       </c>
@@ -8529,7 +9060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:41" ht="25.5" hidden="1">
       <c r="B186" s="7" t="s">
         <v>251</v>
       </c>
@@ -8544,7 +9075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:41" ht="25.5" hidden="1">
       <c r="B187" s="7" t="s">
         <v>253</v>
       </c>
@@ -8559,7 +9090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:41" ht="25.5" hidden="1">
       <c r="B188" s="7" t="s">
         <v>255</v>
       </c>
@@ -8574,7 +9105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:41" ht="25.5" hidden="1">
       <c r="B189" s="7" t="s">
         <v>257</v>
       </c>
@@ -8589,7 +9120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:41" ht="25.5" hidden="1">
       <c r="B190" s="7" t="s">
         <v>259</v>
       </c>
@@ -8604,7 +9135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:41" ht="25.5" hidden="1">
       <c r="B191" s="7" t="s">
         <v>261</v>
       </c>
@@ -8619,7 +9150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:41" ht="25.5" hidden="1">
       <c r="B192" s="7" t="s">
         <v>263</v>
       </c>
@@ -8634,7 +9165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:41" ht="25.5" hidden="1">
       <c r="B193" s="7" t="s">
         <v>266</v>
       </c>
@@ -8649,7 +9180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:41" ht="25.5" hidden="1">
       <c r="B194" s="7" t="s">
         <v>268</v>
       </c>
@@ -8664,7 +9195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="2:41" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:41" ht="25.5" hidden="1">
       <c r="B195" s="7" t="s">
         <v>270</v>
       </c>
@@ -8676,66 +9207,66 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:41">
       <c r="B196" s="7"/>
       <c r="Y196" s="42"/>
     </row>
-    <row r="197" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:41">
       <c r="B197" s="7"/>
       <c r="Y197" s="42"/>
     </row>
-    <row r="198" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:41">
       <c r="B198" s="7"/>
       <c r="Y198" s="42"/>
     </row>
-    <row r="199" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:41">
       <c r="B199" s="7"/>
       <c r="Y199" s="42"/>
     </row>
-    <row r="200" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:41">
       <c r="B200" s="7"/>
     </row>
-    <row r="201" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:41">
       <c r="B201" s="7"/>
     </row>
-    <row r="202" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:41">
       <c r="B202" s="7"/>
     </row>
-    <row r="203" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:41">
       <c r="B203" s="7"/>
     </row>
-    <row r="204" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:41">
       <c r="B204" s="7"/>
     </row>
-    <row r="205" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:41">
       <c r="B205" s="7"/>
     </row>
-    <row r="206" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:41">
       <c r="B206" s="7"/>
     </row>
-    <row r="207" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:41">
       <c r="B207" s="7"/>
     </row>
-    <row r="208" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:41">
       <c r="B208" s="7"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:2">
       <c r="B209" s="7"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:2">
       <c r="B210" s="7"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:2">
       <c r="B211" s="7"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:2">
       <c r="B212" s="7"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:2">
       <c r="B213" s="7"/>
     </row>
-    <row r="5208" spans="7:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5209" spans="7:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5208" spans="7:23" ht="12.75" customHeight="1"/>
+    <row r="5209" spans="7:23" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="AA2:AC2"/>
@@ -8756,12 +9287,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="4.140625" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
@@ -8769,7 +9300,7 @@
     <col min="5" max="5" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" ht="12.75" customHeight="1">
       <c r="B3" s="7" t="s">
         <v>272</v>
       </c>
@@ -8783,7 +9314,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="12.75" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>275</v>
       </c>
@@ -8797,7 +9328,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" ht="12.75" customHeight="1">
       <c r="B5" s="7" t="s">
         <v>277</v>
       </c>

</xml_diff>